<commit_message>
QSAR calculations now conclued.
Parameters files updated

paramters supplementary updated
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFB1541E-541B-4842-A822-BA31DB651BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D786B4D-37AC-4494-8907-D804D3A402EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male " sheetId="1" r:id="rId1"/>
-    <sheet name="Female" sheetId="2" r:id="rId2"/>
+    <sheet name="Partition coefficients" sheetId="3" r:id="rId2"/>
+    <sheet name="Female" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="298">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -948,6 +948,105 @@
   </si>
   <si>
     <t>Fat_Blood partition coefficient  [conc_fat/conc_blood]</t>
+  </si>
+  <si>
+    <t>P_Pu</t>
+  </si>
+  <si>
+    <t>lung:Blood</t>
+  </si>
+  <si>
+    <t>P_PB_Benz</t>
+  </si>
+  <si>
+    <t>1,66*10^4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood:Air </t>
+  </si>
+  <si>
+    <t>P_SP_Benz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slowly perfused tissues:Blood </t>
+  </si>
+  <si>
+    <t>P_RP_Benz</t>
+  </si>
+  <si>
+    <t>Richly perfused tissues:Blood</t>
+  </si>
+  <si>
+    <t>P_SI_Benz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Small intestine:Blood </t>
+  </si>
+  <si>
+    <t>P_L_Benz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liver:Blood </t>
+  </si>
+  <si>
+    <t>P_F_Benz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fat:Blood </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzaldehyde </t>
+  </si>
+  <si>
+    <t>P_OH_Pu</t>
+  </si>
+  <si>
+    <t>P_OH_SP</t>
+  </si>
+  <si>
+    <t>P_OH_RP</t>
+  </si>
+  <si>
+    <t>P_OH_SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_OH_L </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P_OH_F </t>
+  </si>
+  <si>
+    <t>Cinnamyl Alcohol</t>
+  </si>
+  <si>
+    <t>P_PB</t>
+  </si>
+  <si>
+    <t>1,25*10^5</t>
+  </si>
+  <si>
+    <t>P_SP</t>
+  </si>
+  <si>
+    <t>P_RP</t>
+  </si>
+  <si>
+    <t>P_SI</t>
+  </si>
+  <si>
+    <t>P_L</t>
+  </si>
+  <si>
+    <t>P_F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinnamaldehyde </t>
+  </si>
+  <si>
+    <t>Variable name in R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition coefficients </t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1199,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,6 +1253,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1180,6 +1283,18 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C507A35-1641-4240-8A16-960F6A7B0DD2}" name="Tabel1" displayName="Tabel1" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{1365ACB4-3CB9-4795-A16C-DB1A83EDB459}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B02E856B-B775-4096-B9B0-15F38B49912D}" name="Partition coefficients "/>
+    <tableColumn id="2" xr3:uid="{F3959F8A-4253-4F39-84C7-1691EF473EFB}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{303D2048-4430-4751-B883-0219464E8449}" name="Variable name in R"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1481,7 +1596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D684224-74AE-4DFE-B7FF-DE9B6310C4D9}">
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K92" sqref="K92"/>
     </sheetView>
   </sheetViews>
@@ -1516,7 +1631,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="26" t="s">
         <v>232</v>
       </c>
     </row>
@@ -1533,7 +1648,7 @@
       <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1548,7 +1663,7 @@
       <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="26"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1563,7 +1678,7 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="26"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1578,7 +1693,7 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="24"/>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1593,7 +1708,7 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1608,7 +1723,7 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -1623,7 +1738,7 @@
       <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -1638,7 +1753,7 @@
       <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="24"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1653,7 +1768,7 @@
       <c r="D10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1668,7 +1783,7 @@
       <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="24"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -2061,7 +2176,7 @@
       <c r="D36" t="s">
         <v>149</v>
       </c>
-      <c r="E36" s="25" t="s">
+      <c r="E36" s="27" t="s">
         <v>236</v>
       </c>
       <c r="F36" s="12" t="s">
@@ -2081,7 +2196,7 @@
       <c r="D37" t="s">
         <v>149</v>
       </c>
-      <c r="E37" s="25"/>
+      <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
@@ -2124,7 +2239,7 @@
       <c r="D40" t="s">
         <v>159</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="28" t="s">
         <v>238</v>
       </c>
       <c r="F40" s="12" t="s">
@@ -2144,7 +2259,7 @@
       <c r="D41" t="s">
         <v>159</v>
       </c>
-      <c r="E41" s="26"/>
+      <c r="E41" s="28"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
@@ -2188,7 +2303,7 @@
       <c r="D44" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="26" t="s">
         <v>240</v>
       </c>
       <c r="G44" s="6" t="s">
@@ -2208,7 +2323,7 @@
       <c r="D45" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="24"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="6" t="s">
         <v>242</v>
       </c>
@@ -2602,6 +2717,275 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3">
+        <v>1.62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4">
+        <v>0.59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5">
+        <v>0.59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6">
+        <v>0.59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7">
+        <v>0.78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B9">
+        <v>0.59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11">
+        <v>1.64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12">
+        <v>0.59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13">
+        <v>0.59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14">
+        <v>0.59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15">
+        <v>0.78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16">
+        <v>0.59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18">
+        <v>1.51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19">
+        <v>0.59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20">
+        <v>0.59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21">
+        <v>0.59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22">
+        <v>0.78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0.59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CF069-1D83-4C29-B8C9-8D7A85A777EB}">
   <dimension ref="A1:F66"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added sources for pulmonary ventilation and lung mass
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D786B4D-37AC-4494-8907-D804D3A402EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B886393-A840-410B-9D22-F1068AE4B1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male " sheetId="1" r:id="rId1"/>
-    <sheet name="Partition coefficients" sheetId="3" r:id="rId2"/>
-    <sheet name="Female" sheetId="2" r:id="rId3"/>
+    <sheet name="Female" sheetId="2" r:id="rId2"/>
+    <sheet name="Partition coefficients" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="311">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -1047,6 +1047,45 @@
   </si>
   <si>
     <t xml:space="preserve">Partition coefficients </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pop gen </t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>10% up and down of icrp mean for both males and females</t>
+  </si>
+  <si>
+    <t>Annals of the ICRP ICRP PUBLICATION 89 Basic Anatomical and Physiological Data for Use in Radiological Protection: Reference Values</t>
+  </si>
+  <si>
+    <t>Pulmonary ventilation</t>
+  </si>
+  <si>
+    <t>P_V</t>
+  </si>
+  <si>
+    <t>Sitting awake</t>
+  </si>
+  <si>
+    <t>rnorm(N, mean=390, sd=3)</t>
+  </si>
+  <si>
+    <t>99,7 % of the population with the mean pv of woman</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>rnorm(N, mean=540, sd=3)</t>
+  </si>
+  <si>
+    <t>99,7 % of the population with the mean pv of men</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D684224-74AE-4DFE-B7FF-DE9B6310C4D9}">
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView topLeftCell="A117" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2717,280 +2756,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CF069-1D83-4C29-B8C9-8D7A85A777EB}">
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>279</v>
-      </c>
-      <c r="B3">
-        <v>1.62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>277</v>
-      </c>
-      <c r="B4">
-        <v>0.59</v>
-      </c>
-      <c r="C4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>275</v>
-      </c>
-      <c r="B5">
-        <v>0.59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>273</v>
-      </c>
-      <c r="B6">
-        <v>0.59</v>
-      </c>
-      <c r="C6" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B7">
-        <v>0.78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>289</v>
-      </c>
-      <c r="C8" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B9">
-        <v>0.59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11">
-        <v>1.64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B12">
-        <v>0.59</v>
-      </c>
-      <c r="C12" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13">
-        <v>0.59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>273</v>
-      </c>
-      <c r="B14">
-        <v>0.59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>271</v>
-      </c>
-      <c r="B15">
-        <v>0.78</v>
-      </c>
-      <c r="C15" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>266</v>
-      </c>
-      <c r="B16">
-        <v>0.59</v>
-      </c>
-      <c r="C16" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="25" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>279</v>
-      </c>
-      <c r="B18">
-        <v>1.51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>277</v>
-      </c>
-      <c r="B19">
-        <v>0.59</v>
-      </c>
-      <c r="C19" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>275</v>
-      </c>
-      <c r="B20">
-        <v>0.59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>273</v>
-      </c>
-      <c r="B21">
-        <v>0.59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B22">
-        <v>0.78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>269</v>
-      </c>
-      <c r="B23" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="C23" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>266</v>
-      </c>
-      <c r="B24">
-        <v>0.59</v>
-      </c>
-      <c r="C24" t="s">
-        <v>265</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CF069-1D83-4C29-B8C9-8D7A85A777EB}">
-  <dimension ref="A1:F66"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3969,7 +3739,335 @@
         <v>186</v>
       </c>
     </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>298</v>
+      </c>
+      <c r="B94" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B95" t="s">
+        <v>300</v>
+      </c>
+      <c r="C95" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>302</v>
+      </c>
+      <c r="B98" t="s">
+        <v>300</v>
+      </c>
+      <c r="C98" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>307</v>
+      </c>
+      <c r="B101" t="s">
+        <v>305</v>
+      </c>
+      <c r="C101" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>308</v>
+      </c>
+      <c r="B102" t="s">
+        <v>309</v>
+      </c>
+      <c r="C102" t="s">
+        <v>310</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B3">
+        <v>1.62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4">
+        <v>0.59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5">
+        <v>0.59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6">
+        <v>0.59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B7">
+        <v>0.78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>266</v>
+      </c>
+      <c r="B9">
+        <v>0.59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>279</v>
+      </c>
+      <c r="B11">
+        <v>1.64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12">
+        <v>0.59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>275</v>
+      </c>
+      <c r="B13">
+        <v>0.59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>273</v>
+      </c>
+      <c r="B14">
+        <v>0.59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15">
+        <v>0.78</v>
+      </c>
+      <c r="C15" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16">
+        <v>0.59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="25" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>279</v>
+      </c>
+      <c r="B18">
+        <v>1.51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19">
+        <v>0.59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20">
+        <v>0.59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21">
+        <v>0.59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>271</v>
+      </c>
+      <c r="B22">
+        <v>0.78</v>
+      </c>
+      <c r="C22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>269</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B24">
+        <v>0.59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>265</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made sure that changes in the tissue volumes and bloodflows will not mess op the mass balance or exceed Q_C
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6B903F-77F3-4310-B677-ED13426EF0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B6AAA3-B88A-4166-98C3-15939C3DE4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7440" yWindow="3276" windowWidth="17280" windowHeight="8964" tabRatio="860" activeTab="2" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" activeTab="2" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -1771,82 +1771,6 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1939,6 +1863,82 @@
         <bottom style="thin">
           <color theme="5" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -2161,7 +2161,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}" name="Tabel9" displayName="Tabel9" ref="A1:F45" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}" name="Tabel9" displayName="Tabel9" ref="A1:F45" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="A1:F45" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E56BCEE8-B1D6-4C01-83D0-DDF02E730936}" name="Parameter "/>
@@ -2176,7 +2176,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}" name="Tabel911" displayName="Tabel911" ref="A1:F47" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}" name="Tabel911" displayName="Tabel911" ref="A1:F47" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:F47" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0E284C69-B1DD-4E31-A3F5-7CB96E6AF19D}" name="Parameter "/>
@@ -2236,15 +2236,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}" name="Tabel3" displayName="Tabel3" ref="A1:F40" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}" name="Tabel3" displayName="Tabel3" ref="A1:F40" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:F40" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9E6D16AC-BCC0-4871-B66F-97BF63950B51}" name="Parameter "/>
     <tableColumn id="2" xr3:uid="{26DD8215-41B0-459C-A9AE-2F2D7AFDB86E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{14CB4CA6-E35E-4F7D-A582-7A40DA32B9E0}" name="Value"/>
     <tableColumn id="4" xr3:uid="{5EBB9576-9587-4C7D-A236-37CEF71F24E3}" name="Unit "/>
-    <tableColumn id="5" xr3:uid="{EA1BF9BF-3C1D-47A0-98E2-6A086009FE82}" name="Reference " dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{2D8D3B4C-6456-4490-A06B-05F8F69E5369}" name="Notes" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{EA1BF9BF-3C1D-47A0-98E2-6A086009FE82}" name="Reference " dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2D8D3B4C-6456-4490-A06B-05F8F69E5369}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4498,7 +4498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor changes to packages that are loaded.
Global SA made independent and added a write to csv for the Sa parameter distributions to conserve memory
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B6AAA3-B88A-4166-98C3-15939C3DE4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5232AD5-6A89-4EF7-9D40-3FD061D24A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" activeTab="2" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" activeTab="5" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -2562,7 +2562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D684224-74AE-4DFE-B7FF-DE9B6310C4D9}">
   <dimension ref="A1:W96"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -3979,7 +3979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CF069-1D83-4C29-B8C9-8D7A85A777EB}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -4498,7 +4498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A42" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -4619,8 +4619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865D0B40-9BC0-4E55-824F-A8C0062232E1}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:F45"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5024,8 +5024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC645DA-818E-45E2-9276-0EC59E1A8287}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5035,7 +5035,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="32.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Pulmonary vent corrected to BW?
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5232AD5-6A89-4EF7-9D40-3FD061D24A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C63090E-368D-46EF-BC63-130E05CD64D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" activeTab="5" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="3" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="387">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -1522,6 +1522,15 @@
   </si>
   <si>
     <t>var_m_pop$V_B</t>
+  </si>
+  <si>
+    <t>Male: PBW = 50+0.91 × (height in cm–152.4) Kg • Female: PBW = 45.5+0.91 × (height in cm–152.4) Kg</t>
+  </si>
+  <si>
+    <t>Devine B: Gentamicin therapy. Drug Intell Clin Pharm 1974; 8:650–655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ml/kgbw as measur of tidal volume </t>
   </si>
 </sst>
 </file>
@@ -4498,7 +4507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -4617,10 +4626,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865D0B40-9BC0-4E55-824F-A8C0062232E1}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4726,6 +4735,21 @@
       </c>
       <c r="D45" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -5024,7 +5048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC645DA-818E-45E2-9276-0EC59E1A8287}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -5302,7 +5326,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>309</v>
       </c>
@@ -6362,8 +6386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update to parameters and auc calc
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94637BB1-E6EB-4276-A74B-49C3BC624FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4CA79E-7975-4539-A2D4-72DF3B692A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" firstSheet="1" activeTab="6" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="8" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,6 @@
     <sheet name="Partition coefficients" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2544,22 +2543,22 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="102.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="102.109375" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2579,7 +2578,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>271</v>
       </c>
@@ -2591,7 +2590,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>57</v>
       </c>
@@ -2607,7 +2606,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>59</v>
       </c>
@@ -2623,7 +2622,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>64</v>
       </c>
@@ -2639,7 +2638,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>67</v>
       </c>
@@ -2657,7 +2656,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>70</v>
       </c>
@@ -2673,7 +2672,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>74</v>
       </c>
@@ -2689,7 +2688,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>77</v>
       </c>
@@ -2707,7 +2706,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>82</v>
       </c>
@@ -2723,7 +2722,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2741,7 +2740,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2759,7 +2758,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -2775,7 +2774,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -2791,7 +2790,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2809,7 +2808,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -2825,7 +2824,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2841,7 +2840,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="112.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2857,7 +2856,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -2875,7 +2874,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -2893,7 +2892,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>53</v>
       </c>
@@ -2911,7 +2910,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -2949,7 +2948,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -2967,7 +2966,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -3006,7 +3005,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>238</v>
       </c>
@@ -3029,7 +3028,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -3040,7 +3039,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3051,7 +3050,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3062,7 +3061,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3073,7 +3072,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3084,7 +3083,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3095,7 +3094,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3106,7 +3105,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3117,7 +3116,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -3128,7 +3127,7 @@
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -3139,7 +3138,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -3150,7 +3149,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3161,7 +3160,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -3172,7 +3171,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3183,7 +3182,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -3194,7 +3193,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3205,7 +3204,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3216,7 +3215,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3227,7 +3226,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -3238,7 +3237,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3249,7 +3248,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -3260,7 +3259,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -3271,7 +3270,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -3282,7 +3281,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3293,7 +3292,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3304,8 +3303,8 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3316,7 +3315,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -3327,7 +3326,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -3338,8 +3337,8 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -3350,7 +3349,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -3361,7 +3360,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3372,8 +3371,8 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -3384,7 +3383,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -3395,7 +3394,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -3406,7 +3405,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -3417,8 +3416,8 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -3429,7 +3428,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -3440,7 +3439,7 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -3451,7 +3450,7 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -3462,7 +3461,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -3473,7 +3472,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -3484,7 +3483,7 @@
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -3495,7 +3494,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -3506,7 +3505,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -3517,7 +3516,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -3528,7 +3527,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -3539,7 +3538,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -3550,7 +3549,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -3561,7 +3560,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -3572,7 +3571,7 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -3583,7 +3582,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -3594,7 +3593,7 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -3619,7 +3618,7 @@
       <c r="V83" s="13"/>
       <c r="W83" s="13"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -3644,7 +3643,7 @@
       <c r="V84" s="13"/>
       <c r="W84" s="13"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -3669,7 +3668,7 @@
       <c r="V85" s="13"/>
       <c r="W85" s="13"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -3694,7 +3693,7 @@
       <c r="V86" s="13"/>
       <c r="W86" s="13"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="32"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -3719,7 +3718,7 @@
       <c r="V87" s="13"/>
       <c r="W87" s="13"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3744,7 +3743,7 @@
       <c r="V88" s="13"/>
       <c r="W88" s="13"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -3769,7 +3768,7 @@
       <c r="V89" s="13"/>
       <c r="W89" s="13"/>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -3794,7 +3793,7 @@
       <c r="V90" s="13"/>
       <c r="W90" s="13"/>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -3819,7 +3818,7 @@
       <c r="V91" s="13"/>
       <c r="W91" s="13"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -3844,7 +3843,7 @@
       <c r="V92" s="13"/>
       <c r="W92" s="13"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -3869,7 +3868,7 @@
       <c r="V93" s="13"/>
       <c r="W93" s="13"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -3894,7 +3893,7 @@
       <c r="V94" s="13"/>
       <c r="W94" s="13"/>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -3919,7 +3918,7 @@
       <c r="V95" s="13"/>
       <c r="W95" s="13"/>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -3961,17 +3960,17 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="108.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="108.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3991,14 +3990,14 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>254</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -4057,7 +4056,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -4085,7 +4084,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -4102,7 +4101,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -4116,13 +4115,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>253</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4139,7 +4138,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -4170,7 +4169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -4187,7 +4186,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -4204,7 +4203,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -4218,7 +4217,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4232,7 +4231,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4246,7 +4245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -4266,7 +4265,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -4283,13 +4282,13 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>250</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -4306,7 +4305,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -4326,7 +4325,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -4371,7 +4370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -4385,7 +4384,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>238</v>
       </c>
@@ -4405,7 +4404,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>233</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>235</v>
       </c>
@@ -4421,12 +4420,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>237</v>
       </c>
@@ -4437,12 +4436,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>242</v>
       </c>
@@ -4453,7 +4452,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>243</v>
       </c>
@@ -4476,20 +4475,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4509,17 +4508,17 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>357</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>369</v>
       </c>
@@ -4556,7 +4555,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>368</v>
       </c>
@@ -4570,7 +4569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>367</v>
       </c>
@@ -4601,17 +4600,17 @@
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4631,17 +4630,17 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>353</v>
       </c>
@@ -4661,7 +4660,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>359</v>
       </c>
@@ -4678,7 +4677,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>363</v>
       </c>
@@ -4692,7 +4691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -4706,17 +4705,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>372</v>
       </c>
@@ -4738,17 +4737,17 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -4782,7 +4781,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>275</v>
       </c>
@@ -4790,7 +4789,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -4801,7 +4800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -4812,7 +4811,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>288</v>
       </c>
@@ -4834,7 +4833,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>286</v>
       </c>
@@ -4856,7 +4855,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>285</v>
       </c>
@@ -4867,7 +4866,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>284</v>
       </c>
@@ -4878,12 +4877,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -4897,7 +4896,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>300</v>
       </c>
@@ -4911,7 +4910,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>299</v>
       </c>
@@ -4925,7 +4924,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>298</v>
       </c>
@@ -4939,7 +4938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>297</v>
       </c>
@@ -4953,7 +4952,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>296</v>
       </c>
@@ -4967,7 +4966,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>295</v>
       </c>
@@ -4984,7 +4983,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>294</v>
       </c>
@@ -5021,17 +5020,17 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="32.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="32.5546875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5051,7 +5050,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>273</v>
       </c>
@@ -5068,7 +5067,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>275</v>
       </c>
@@ -5076,7 +5075,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -5090,7 +5089,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -5118,7 +5117,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>288</v>
       </c>
@@ -5132,7 +5131,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -5146,7 +5145,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>286</v>
       </c>
@@ -5160,7 +5159,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>285</v>
       </c>
@@ -5174,7 +5173,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>284</v>
       </c>
@@ -5188,12 +5187,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -5210,7 +5209,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>300</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>299</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>298</v>
       </c>
@@ -5261,7 +5260,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>297</v>
       </c>
@@ -5278,7 +5277,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>296</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>295</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>238</v>
       </c>
@@ -5347,22 +5346,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227D4F3-7485-4534-9D8C-979B86ED3B4D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5383,7 +5382,7 @@
       </c>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>251</v>
       </c>
@@ -5392,7 +5391,7 @@
       </c>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5411,7 +5410,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -5430,7 +5429,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:7" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5448,7 +5447,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5466,7 +5465,7 @@
       </c>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:7" ht="182.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -5485,7 +5484,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -5504,7 +5503,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -5519,7 +5518,7 @@
       </c>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:7" ht="169.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>252</v>
       </c>
@@ -5528,11 +5527,11 @@
       </c>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5553,7 +5552,7 @@
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -5574,7 +5573,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="31" t="s">
         <v>266</v>
       </c>
@@ -5585,7 +5584,7 @@
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -5606,7 +5605,7 @@
       </c>
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -5615,7 +5614,7 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -5636,19 +5635,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC505D8B-0BF3-4962-BD98-F6AA5F552AB5}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A24" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5668,7 +5667,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>307</v>
       </c>
@@ -5678,7 +5677,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>160</v>
       </c>
@@ -5696,7 +5695,7 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>163</v>
       </c>
@@ -5714,7 +5713,7 @@
       </c>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>167</v>
       </c>
@@ -5732,7 +5731,7 @@
       </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>168</v>
       </c>
@@ -5750,7 +5749,7 @@
       </c>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>169</v>
       </c>
@@ -5768,7 +5767,7 @@
       </c>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>170</v>
       </c>
@@ -5786,7 +5785,7 @@
       </c>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>171</v>
       </c>
@@ -5804,7 +5803,7 @@
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>172</v>
       </c>
@@ -5822,7 +5821,7 @@
       </c>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>173</v>
       </c>
@@ -5840,7 +5839,7 @@
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>174</v>
       </c>
@@ -5858,7 +5857,7 @@
       </c>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>246</v>
       </c>
@@ -5876,7 +5875,7 @@
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>175</v>
       </c>
@@ -5894,7 +5893,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>247</v>
       </c>
@@ -5912,7 +5911,7 @@
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>177</v>
       </c>
@@ -5930,7 +5929,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>179</v>
       </c>
@@ -5948,7 +5947,7 @@
       </c>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>180</v>
       </c>
@@ -5966,7 +5965,7 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>182</v>
       </c>
@@ -5984,7 +5983,7 @@
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>183</v>
       </c>
@@ -6002,17 +6001,17 @@
       </c>
       <c r="F20" s="26"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>308</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E23" s="28"/>
     </row>
-    <row r="24" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>309</v>
       </c>
@@ -6030,7 +6029,7 @@
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>163</v>
       </c>
@@ -6047,7 +6046,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>313</v>
       </c>
@@ -6065,7 +6064,7 @@
       </c>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>314</v>
       </c>
@@ -6082,7 +6081,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>316</v>
       </c>
@@ -6100,7 +6099,7 @@
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>317</v>
       </c>
@@ -6117,7 +6116,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>318</v>
       </c>
@@ -6135,7 +6134,7 @@
       </c>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>319</v>
       </c>
@@ -6152,7 +6151,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>320</v>
       </c>
@@ -6170,7 +6169,7 @@
       </c>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>321</v>
       </c>
@@ -6187,7 +6186,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>322</v>
       </c>
@@ -6205,7 +6204,7 @@
       </c>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>311</v>
       </c>
@@ -6222,7 +6221,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>323</v>
       </c>
@@ -6240,7 +6239,7 @@
       </c>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>324</v>
       </c>
@@ -6257,7 +6256,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>325</v>
       </c>
@@ -6275,7 +6274,7 @@
       </c>
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>326</v>
       </c>
@@ -6292,7 +6291,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>327</v>
       </c>
@@ -6310,7 +6309,7 @@
       </c>
       <c r="F40" s="14"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="36"/>
       <c r="B45" s="36"/>
       <c r="D45" s="36"/>
@@ -6327,19 +6326,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>232</v>
       </c>
@@ -6353,7 +6352,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>343</v>
       </c>
@@ -6361,7 +6360,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -6375,7 +6374,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>215</v>
       </c>
@@ -6389,7 +6388,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>213</v>
       </c>
@@ -6403,7 +6402,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -6431,7 +6430,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>207</v>
       </c>
@@ -6445,7 +6444,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>204</v>
       </c>
@@ -6459,7 +6458,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>345</v>
       </c>
@@ -6467,7 +6466,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>217</v>
       </c>
@@ -6481,7 +6480,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -6495,7 +6494,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>213</v>
       </c>
@@ -6509,7 +6508,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>211</v>
       </c>
@@ -6523,7 +6522,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>209</v>
       </c>
@@ -6537,7 +6536,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>204</v>
       </c>
@@ -6551,7 +6550,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>344</v>
       </c>
@@ -6559,7 +6558,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>217</v>
       </c>
@@ -6573,7 +6572,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -6587,7 +6586,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>213</v>
       </c>
@@ -6601,7 +6600,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>211</v>
       </c>
@@ -6615,7 +6614,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>209</v>
       </c>
@@ -6629,7 +6628,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>207</v>
       </c>
@@ -6643,7 +6642,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>204</v>
       </c>
@@ -6657,7 +6656,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>232</v>
       </c>
@@ -6671,7 +6670,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>347</v>
       </c>
@@ -6679,7 +6678,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -6693,7 +6692,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -6707,7 +6706,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>213</v>
       </c>
@@ -6721,7 +6720,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>211</v>
       </c>
@@ -6735,7 +6734,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>209</v>
       </c>
@@ -6749,7 +6748,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>207</v>
       </c>
@@ -6763,7 +6762,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>204</v>
       </c>
@@ -6777,7 +6776,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>348</v>
       </c>
@@ -6785,7 +6784,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>217</v>
       </c>
@@ -6799,7 +6798,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>215</v>
       </c>
@@ -6813,7 +6812,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>213</v>
       </c>
@@ -6827,7 +6826,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -6841,7 +6840,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>209</v>
       </c>
@@ -6855,7 +6854,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -6869,7 +6868,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>349</v>
       </c>
@@ -6877,7 +6876,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>217</v>
       </c>
@@ -6891,7 +6890,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>215</v>
       </c>
@@ -6905,7 +6904,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>213</v>
       </c>
@@ -6919,7 +6918,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -6933,7 +6932,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>209</v>
       </c>
@@ -6947,7 +6946,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>207</v>
       </c>
@@ -6961,7 +6960,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>204</v>
       </c>

</xml_diff>

<commit_message>
Found an error in how PC where calculated fixed this error. (not properly log transformed.)
added some calculations to the data processing file
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4CA79E-7975-4539-A2D4-72DF3B692A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC9CEFA-1ED9-4D4D-B926-0F87BB084552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="8" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
@@ -6326,7 +6326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed a wrong blood air parttion coefficient
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC9CEFA-1ED9-4D4D-B926-0F87BB084552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B93206-B3EC-4DBB-A8CD-2A2077FFF90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="8" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="383">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -1402,9 +1402,6 @@
     <t>Cinnamaldehyde Human</t>
   </si>
   <si>
-    <t>Benzaldehyde Human</t>
-  </si>
-  <si>
     <t>Cinnamyl Alcohol Human</t>
   </si>
   <si>
@@ -1503,12 +1500,39 @@
   <si>
     <t>A value of 5319 umol/kg is noted in the paper not 3000 as can be seen in Kiwamoto et al</t>
   </si>
+  <si>
+    <t xml:space="preserve">cinnmaldehyde vapor </t>
+  </si>
+  <si>
+    <t>Q: 0,0337 mm Hg</t>
+  </si>
+  <si>
+    <t>Q: 2,15E+03 mg/L</t>
+  </si>
+  <si>
+    <t>cinnmaldehyde solubility</t>
+  </si>
+  <si>
+    <t>25 c</t>
+  </si>
+  <si>
+    <t>3,54E-06 atm-m3/mole</t>
+  </si>
+  <si>
+    <t>Epitsuite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Henry's law constant </t>
+  </si>
+  <si>
+    <t>Benzaldehyde Human (Wrong)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1580,6 +1604,14 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1670,7 +1702,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1740,6 +1772,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -2083,6 +2116,143 @@
         <a:xfrm>
           <a:off x="0" y="579120"/>
           <a:ext cx="4686300" cy="6766560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>593060</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>244929</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95476</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>535380</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Afbeelding 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2C6D2D9-6744-E030-018D-3E6AAC2CD918}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12164574" y="429986"/>
+          <a:ext cx="3769616" cy="2500251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>246598</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>221919</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>108485</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>68430</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Afbeelding 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF2E897B-135E-DBAA-FEF7-AD2A74B5A594}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8770112" y="5174919"/>
+          <a:ext cx="4738687" cy="1501140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>445226</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>211785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>365400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>697930</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Afbeelding 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{060AB7E2-C9E8-EC64-DA25-B61BF40C2CCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7749540" y="396842"/>
+          <a:ext cx="4187374" cy="2695945"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4510,23 +4680,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4535,18 +4705,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4557,13 +4727,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -4571,13 +4741,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -4632,23 +4802,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>237</v>
       </c>
       <c r="C42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4657,18 +4827,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4679,13 +4849,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -4693,13 +4863,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -4707,17 +4877,17 @@
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
   </sheetData>
@@ -5405,7 +5575,7 @@
         <v>133</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="30"/>
@@ -5424,7 +5594,7 @@
         <v>133</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="30"/>
@@ -5443,7 +5613,7 @@
         <v>161</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G5" s="30"/>
     </row>
@@ -5461,7 +5631,7 @@
         <v>161</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G6" s="30"/>
     </row>
@@ -5479,7 +5649,7 @@
         <v>142</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="30"/>
@@ -5498,7 +5668,7 @@
         <v>142</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="30"/>
@@ -5548,7 +5718,7 @@
         <v>200</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G12" s="30"/>
     </row>
@@ -6324,10 +6494,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6349,7 +6519,7 @@
         <v>231</v>
       </c>
       <c r="D1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -6365,7 +6535,7 @@
         <v>217</v>
       </c>
       <c r="B3">
-        <v>1.62</v>
+        <v>47.75</v>
       </c>
       <c r="C3" t="s">
         <v>230</v>
@@ -6379,7 +6549,7 @@
         <v>215</v>
       </c>
       <c r="B4">
-        <v>0.59</v>
+        <v>1.83</v>
       </c>
       <c r="C4" t="s">
         <v>229</v>
@@ -6393,7 +6563,7 @@
         <v>213</v>
       </c>
       <c r="B5">
-        <v>0.59</v>
+        <v>1.81</v>
       </c>
       <c r="C5" t="s">
         <v>228</v>
@@ -6407,7 +6577,7 @@
         <v>211</v>
       </c>
       <c r="B6">
-        <v>0.59</v>
+        <v>1.81</v>
       </c>
       <c r="C6" t="s">
         <v>227</v>
@@ -6421,7 +6591,7 @@
         <v>209</v>
       </c>
       <c r="B7">
-        <v>0.78</v>
+        <v>1.5</v>
       </c>
       <c r="C7" t="s">
         <v>226</v>
@@ -6434,8 +6604,8 @@
       <c r="A8" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>225</v>
+      <c r="B8" s="9">
+        <v>0.28999999999999998</v>
       </c>
       <c r="C8" t="s">
         <v>224</v>
@@ -6449,7 +6619,7 @@
         <v>204</v>
       </c>
       <c r="B9">
-        <v>0.59</v>
+        <v>1.81</v>
       </c>
       <c r="C9" t="s">
         <v>203</v>
@@ -6460,7 +6630,7 @@
     </row>
     <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>264</v>
@@ -6471,7 +6641,7 @@
         <v>217</v>
       </c>
       <c r="B11">
-        <v>1.64</v>
+        <v>49.26</v>
       </c>
       <c r="C11" t="s">
         <v>223</v>
@@ -6485,7 +6655,7 @@
         <v>215</v>
       </c>
       <c r="B12">
-        <v>0.59</v>
+        <v>1.18</v>
       </c>
       <c r="C12" t="s">
         <v>222</v>
@@ -6499,7 +6669,7 @@
         <v>213</v>
       </c>
       <c r="B13">
-        <v>0.59</v>
+        <v>1.18</v>
       </c>
       <c r="C13" t="s">
         <v>221</v>
@@ -6513,7 +6683,7 @@
         <v>211</v>
       </c>
       <c r="B14">
-        <v>0.59</v>
+        <v>1.18</v>
       </c>
       <c r="C14" t="s">
         <v>220</v>
@@ -6527,7 +6697,7 @@
         <v>209</v>
       </c>
       <c r="B15">
-        <v>0.78</v>
+        <v>1.53</v>
       </c>
       <c r="C15" t="s">
         <v>219</v>
@@ -6541,7 +6711,7 @@
         <v>204</v>
       </c>
       <c r="B16">
-        <v>0.59</v>
+        <v>1.18</v>
       </c>
       <c r="C16" t="s">
         <v>218</v>
@@ -6551,8 +6721,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>344</v>
+      <c r="A17" s="39" t="s">
+        <v>382</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>264</v>
@@ -6667,12 +6837,12 @@
         <v>231</v>
       </c>
       <c r="D26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>264</v>
@@ -6778,7 +6948,7 @@
     </row>
     <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>264</v>
@@ -6870,7 +7040,7 @@
     </row>
     <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>264</v>
@@ -6974,11 +7144,51 @@
         <v>264</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>374</v>
+      </c>
+      <c r="B55" t="s">
+        <v>375</v>
+      </c>
+      <c r="D55" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>377</v>
+      </c>
+      <c r="B56" t="s">
+        <v>376</v>
+      </c>
+      <c r="D56" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>381</v>
+      </c>
+      <c r="B57" t="s">
+        <v>379</v>
+      </c>
+      <c r="D57" t="s">
+        <v>380</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pc to lung was wrong
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E782C3FA-E674-4D2A-B237-BBDE2982FF8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AE4608-995B-4160-A101-1B7A295185F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="8" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
@@ -1411,9 +1411,6 @@
     <t>Cinnamyl Alcohol Rat</t>
   </si>
   <si>
-    <t>Benzaldehyde Rat</t>
-  </si>
-  <si>
     <t>Generation parameters Male in Popgen</t>
   </si>
   <si>
@@ -1523,6 +1520,9 @@
   </si>
   <si>
     <t>Benzaldehyde Human (Wrong)</t>
+  </si>
+  <si>
+    <t>Benzaldehyde Rat (Wrong)</t>
   </si>
 </sst>
 </file>
@@ -2172,15 +2172,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>246598</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>221919</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>344570</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1125433</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>108485</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>206457</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>68430</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2204,7 +2204,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8770112" y="5174919"/>
+          <a:off x="7648884" y="3520290"/>
           <a:ext cx="4738687" cy="1501140"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -4677,23 +4677,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>236</v>
       </c>
       <c r="C42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4702,18 +4702,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4724,13 +4724,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -4738,13 +4738,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -4799,23 +4799,23 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>236</v>
       </c>
       <c r="C42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4824,18 +4824,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4846,13 +4846,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
@@ -4860,13 +4860,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -4874,17 +4874,17 @@
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5572,7 +5572,7 @@
         <v>133</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="30"/>
@@ -5591,7 +5591,7 @@
         <v>133</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="30"/>
@@ -5610,7 +5610,7 @@
         <v>161</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G5" s="30"/>
     </row>
@@ -5628,7 +5628,7 @@
         <v>161</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G6" s="30"/>
     </row>
@@ -5646,7 +5646,7 @@
         <v>142</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="30"/>
@@ -5665,7 +5665,7 @@
         <v>142</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="30"/>
@@ -5715,7 +5715,7 @@
         <v>200</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="G12" s="30"/>
     </row>
@@ -6493,8 +6493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6719,7 +6719,7 @@
     </row>
     <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>263</v>
@@ -6920,7 +6920,7 @@
         <v>207</v>
       </c>
       <c r="B33" s="9">
-        <v>0.28999999999999998</v>
+        <v>1.81</v>
       </c>
       <c r="C33" t="s">
         <v>224</v>
@@ -7026,7 +7026,7 @@
         <v>204</v>
       </c>
       <c r="B41">
-        <v>0.81</v>
+        <v>1.81</v>
       </c>
       <c r="C41" t="s">
         <v>218</v>
@@ -7036,8 +7036,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10" t="s">
-        <v>347</v>
+      <c r="A42" s="39" t="s">
+        <v>381</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>263</v>
@@ -7143,40 +7143,40 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>372</v>
+      </c>
+      <c r="B55" t="s">
         <v>373</v>
       </c>
-      <c r="B55" t="s">
-        <v>374</v>
-      </c>
       <c r="D55" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B56" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D56" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B57" t="s">
+        <v>377</v>
+      </c>
+      <c r="D57" t="s">
         <v>378</v>
-      </c>
-      <c r="D57" t="s">
-        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed AM_SI_GST in humans as this was zero.
Fixed outcomes of the population model to more acurately correspond to in vivo data
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6783046C-8139-49C8-A915-138860962D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63A532A-9A32-4947-A9B5-2D0E799741C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="4" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" firstSheet="1" activeTab="5" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -738,9 +738,6 @@
 https://doi.org/10.1016/0378-4274(92)90031-E. (https://www.sciencedirect.com/science/article/pii/037842749290031E)</t>
   </si>
   <si>
-    <t xml:space="preserve">A value of 245 umol/kg is noted in the paper not </t>
-  </si>
-  <si>
     <t>This is the remaning slowly perfused tissue after subtracting other slowly perfused compartments</t>
   </si>
   <si>
@@ -1497,6 +1494,9 @@
 Peff.cm.per.hr = Peff.cm.power.minus.four.per.s/10000*3600
 Ka= (Peff.cm.per.hr*2)/R
 Fa = 1-(1+Ka/kt)**-7</t>
+  </si>
+  <si>
+    <t>A value of 245 umol/kg is noted in the paper</t>
   </si>
 </sst>
 </file>
@@ -2051,13 +2051,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>11429</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1059180</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>100524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2085,8 +2085,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="579120"/>
-          <a:ext cx="4686300" cy="6766560"/>
+          <a:off x="0" y="582929"/>
+          <a:ext cx="10410825" cy="15976795"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2684,22 +2684,22 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="102.109375" customWidth="1"/>
-    <col min="3" max="3" width="61.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="102.140625" customWidth="1"/>
+    <col min="3" max="3" width="61.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="6" max="6" width="38.88671875" customWidth="1"/>
-    <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2716,22 +2716,22 @@
         <v>186</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>57</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>59</v>
       </c>
@@ -2763,7 +2763,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>64</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>67</v>
       </c>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>70</v>
       </c>
@@ -2813,7 +2813,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
         <v>74</v>
       </c>
@@ -2829,7 +2829,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>77</v>
       </c>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>82</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2881,7 +2881,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -2915,7 +2915,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -2931,7 +2931,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -2965,7 +2965,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2981,7 +2981,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="112.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2997,7 +2997,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3011,11 +3011,11 @@
         <v>6</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>53</v>
       </c>
@@ -3051,7 +3051,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -3089,7 +3089,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -3107,7 +3107,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -3146,15 +3146,15 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C27" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>35</v>
@@ -3163,13 +3163,13 @@
         <v>193</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -3180,7 +3180,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3191,7 +3191,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3202,7 +3202,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3213,7 +3213,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3224,7 +3224,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3235,7 +3235,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3246,7 +3246,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3257,7 +3257,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -3268,7 +3268,7 @@
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -3279,7 +3279,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -3290,7 +3290,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3301,7 +3301,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -3312,7 +3312,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3323,7 +3323,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -3334,7 +3334,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3345,7 +3345,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3356,7 +3356,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3367,7 +3367,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -3378,7 +3378,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3389,7 +3389,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -3400,7 +3400,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -3411,7 +3411,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -3422,7 +3422,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3433,7 +3433,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3444,8 +3444,8 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3456,7 +3456,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -3467,7 +3467,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -3478,8 +3478,8 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -3490,7 +3490,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -3501,7 +3501,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3512,8 +3512,8 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -3524,7 +3524,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -3535,7 +3535,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -3546,7 +3546,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -3557,8 +3557,8 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -3569,7 +3569,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -3580,7 +3580,7 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -3591,7 +3591,7 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -3602,7 +3602,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -3613,7 +3613,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -3624,7 +3624,7 @@
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -3635,7 +3635,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -3646,7 +3646,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -3657,7 +3657,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -3668,7 +3668,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -3679,7 +3679,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -3690,7 +3690,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -3701,7 +3701,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -3712,7 +3712,7 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -3723,7 +3723,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -3734,7 +3734,7 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -3759,7 +3759,7 @@
       <c r="V83" s="13"/>
       <c r="W83" s="13"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -3784,7 +3784,7 @@
       <c r="V84" s="13"/>
       <c r="W84" s="13"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -3809,7 +3809,7 @@
       <c r="V85" s="13"/>
       <c r="W85" s="13"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -3834,7 +3834,7 @@
       <c r="V86" s="13"/>
       <c r="W86" s="13"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" s="32"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -3859,7 +3859,7 @@
       <c r="V87" s="13"/>
       <c r="W87" s="13"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3884,7 +3884,7 @@
       <c r="V88" s="13"/>
       <c r="W88" s="13"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -3909,7 +3909,7 @@
       <c r="V89" s="13"/>
       <c r="W89" s="13"/>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -3934,7 +3934,7 @@
       <c r="V90" s="13"/>
       <c r="W90" s="13"/>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -3959,7 +3959,7 @@
       <c r="V91" s="13"/>
       <c r="W91" s="13"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -3984,7 +3984,7 @@
       <c r="V92" s="13"/>
       <c r="W92" s="13"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -4009,7 +4009,7 @@
       <c r="V93" s="13"/>
       <c r="W93" s="13"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -4034,7 +4034,7 @@
       <c r="V94" s="13"/>
       <c r="W94" s="13"/>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -4059,7 +4059,7 @@
       <c r="V95" s="13"/>
       <c r="W95" s="13"/>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -4097,21 +4097,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B8CF069-1D83-4C29-B8C9-8D7A85A777EB}">
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" customWidth="1"/>
-    <col min="2" max="2" width="62.109375" customWidth="1"/>
-    <col min="3" max="3" width="108.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="56.5546875" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="62.140625" customWidth="1"/>
+    <col min="3" max="3" width="108.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4128,17 +4128,17 @@
         <v>186</v>
       </c>
       <c r="F1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -4256,13 +4256,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4372,7 +4372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4386,7 +4386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -4406,7 +4406,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -4420,16 +4420,16 @@
         <v>6</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -4446,7 +4446,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -4525,15 +4525,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B29" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D29" t="s">
         <v>35</v>
@@ -4542,66 +4542,66 @@
         <v>193</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>230</v>
+      </c>
+      <c r="B99" t="s">
         <v>231</v>
       </c>
-      <c r="B99" t="s">
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>233</v>
       </c>
-      <c r="C100" t="s">
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B102" t="s">
+      <c r="B103" t="s">
+        <v>232</v>
+      </c>
+      <c r="C103" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>235</v>
-      </c>
-      <c r="B103" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B104" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>239</v>
+      </c>
+      <c r="B106" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+      <c r="C106" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>240</v>
       </c>
-      <c r="B106" t="s">
-        <v>238</v>
-      </c>
-      <c r="C106" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+      <c r="B107" t="s">
         <v>241</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>242</v>
-      </c>
-      <c r="C107" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -4616,20 +4616,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4646,28 +4646,28 @@
         <v>186</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4676,18 +4676,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4696,29 +4696,29 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -4737,21 +4737,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865D0B40-9BC0-4E55-824F-A8C0062232E1}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.88671875" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4768,28 +4768,28 @@
         <v>186</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>347</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" t="s">
         <v>346</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>348</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C42" t="s">
-        <v>347</v>
       </c>
       <c r="D42" t="s">
         <v>35</v>
@@ -4798,18 +4798,18 @@
         <v>193</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B43" t="s">
         <v>109</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
@@ -4818,47 +4818,47 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B44" t="s">
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B45" t="s">
         <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>366</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -4874,21 +4874,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA63B1E-9727-458D-B78C-352DAEF35D45}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="54.28515625" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4905,15 +4905,15 @@
         <v>186</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" t="s">
         <v>270</v>
-      </c>
-      <c r="B2" t="s">
-        <v>271</v>
       </c>
       <c r="C2">
         <v>0.25</v>
@@ -4922,110 +4922,110 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" t="s">
         <v>272</v>
-      </c>
-      <c r="D3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>287</v>
-      </c>
-      <c r="B4" t="s">
-        <v>273</v>
       </c>
       <c r="C4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5">
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6">
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7">
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8">
         <v>5.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C9">
         <v>3.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10">
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C11">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -5037,12 +5037,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14">
         <v>7.0000000000000007E-2</v>
@@ -5051,12 +5051,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15">
         <v>0.13</v>
@@ -5065,12 +5065,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16">
         <v>0.12</v>
@@ -5079,12 +5079,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C17">
         <v>0.64</v>
@@ -5093,12 +5093,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C18">
         <v>0.17</v>
@@ -5107,29 +5107,29 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" t="s">
         <v>289</v>
-      </c>
-      <c r="C19" t="s">
-        <v>290</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B20" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C20">
         <v>0.75</v>
@@ -5138,15 +5138,15 @@
         <v>35</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B21" s="30"/>
       <c r="C21" s="30"/>
@@ -5154,7 +5154,7 @@
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
-    <row r="22" spans="1:6" ht="294.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="294.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>155</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>198</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -5185,21 +5185,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC645DA-818E-45E2-9276-0EC59E1A8287}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="42.85546875" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5216,15 +5216,15 @@
         <v>186</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" t="s">
         <v>270</v>
-      </c>
-      <c r="B2" t="s">
-        <v>271</v>
       </c>
       <c r="C2">
         <v>70</v>
@@ -5236,134 +5236,134 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="D3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" t="s">
         <v>272</v>
-      </c>
-      <c r="D3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>287</v>
-      </c>
-      <c r="B4" t="s">
-        <v>273</v>
       </c>
       <c r="C4">
         <v>21.42</v>
       </c>
       <c r="E4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C5">
         <v>2.57</v>
       </c>
       <c r="E5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C6">
         <v>0.91</v>
       </c>
       <c r="E6" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C8">
         <v>5.9</v>
       </c>
       <c r="E8" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C9">
         <v>4.8</v>
       </c>
       <c r="E9" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C10">
         <v>61.64</v>
       </c>
       <c r="E10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C11">
         <v>0.76</v>
       </c>
       <c r="E11" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B13" t="s">
         <v>36</v>
@@ -5375,15 +5375,15 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C14">
         <v>5.2</v>
@@ -5392,15 +5392,15 @@
         <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C15">
         <v>14.1</v>
@@ -5409,15 +5409,15 @@
         <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B16" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C16">
         <v>8.6</v>
@@ -5426,15 +5426,15 @@
         <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C17">
         <v>47.3</v>
@@ -5443,15 +5443,15 @@
         <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C18">
         <v>24.8</v>
@@ -5460,35 +5460,35 @@
         <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B19" t="s">
+        <v>288</v>
+      </c>
+      <c r="C19" t="s">
         <v>289</v>
-      </c>
-      <c r="C19" t="s">
-        <v>290</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C20">
         <v>540</v>
@@ -5500,10 +5500,10 @@
         <v>193</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="374.4" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="345" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>198</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -5533,22 +5533,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227D4F3-7485-4534-9D8C-979B86ED3B4D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F15"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
-    <col min="5" max="5" width="72.33203125" customWidth="1"/>
-    <col min="6" max="6" width="41.109375" customWidth="1"/>
-    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="72.28515625" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5565,20 +5565,20 @@
         <v>186</v>
       </c>
       <c r="F1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5592,12 +5592,12 @@
         <v>133</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -5611,12 +5611,12 @@
         <v>133</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:7" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5630,11 +5630,11 @@
         <v>161</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5648,11 +5648,11 @@
         <v>161</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:7" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="182.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -5666,12 +5666,12 @@
         <v>142</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -5685,12 +5685,12 @@
         <v>142</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F8" s="4"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -5705,20 +5705,20 @@
       </c>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="169.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5735,11 +5735,11 @@
         <v>199</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -5756,17 +5756,17 @@
         <v>199</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>200</v>
+        <v>381</v>
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -5775,7 +5775,7 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -5796,19 +5796,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC505D8B-0BF3-4962-BD98-F6AA5F552AB5}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="87.6640625" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="87.7109375" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5825,12 +5825,12 @@
         <v>186</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -5838,7 +5838,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>160</v>
       </c>
@@ -5849,14 +5849,14 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>163</v>
       </c>
@@ -5867,32 +5867,32 @@
         <v>8.5</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>167</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C5" s="15">
         <v>330</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>168</v>
       </c>
@@ -5903,32 +5903,32 @@
         <v>100</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>169</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C7" s="22">
         <v>100</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>170</v>
       </c>
@@ -5939,14 +5939,14 @@
         <v>9.6999999999999993</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>171</v>
       </c>
@@ -5957,14 +5957,14 @@
         <v>73</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>172</v>
       </c>
@@ -5975,14 +5975,14 @@
         <v>37</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>173</v>
       </c>
@@ -5993,14 +5993,14 @@
         <v>100</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>174</v>
       </c>
@@ -6011,32 +6011,32 @@
         <v>70</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C13" s="15">
         <v>90</v>
       </c>
       <c r="D13" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>175</v>
       </c>
@@ -6047,16 +6047,16 @@
         <v>290</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>176</v>
@@ -6065,32 +6065,32 @@
         <v>600</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>177</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C16" s="14">
         <v>100</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>179</v>
       </c>
@@ -6101,32 +6101,32 @@
         <v>21</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>180</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C18" s="14">
         <v>30</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>182</v>
       </c>
@@ -6137,14 +6137,14 @@
         <v>5</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>183</v>
       </c>
@@ -6155,322 +6155,322 @@
         <v>63</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F20" s="26"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E23" s="28"/>
     </row>
-    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B24" t="s">
         <v>306</v>
-      </c>
-      <c r="B24" t="s">
-        <v>307</v>
       </c>
       <c r="C24">
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>163</v>
       </c>
       <c r="B25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C25">
         <v>8.5</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B26" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C26">
         <v>330</v>
       </c>
       <c r="D26" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C27">
         <v>100</v>
       </c>
       <c r="D27" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C28">
         <v>17000</v>
       </c>
       <c r="D28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C29">
         <v>9.6999999999999993</v>
       </c>
       <c r="D29" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C30">
         <v>73</v>
       </c>
       <c r="D30" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C31">
         <v>37</v>
       </c>
       <c r="D31" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C32">
         <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C33">
         <v>90</v>
       </c>
       <c r="D33" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B34" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C34">
         <v>290</v>
       </c>
       <c r="D34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C35">
         <v>600</v>
       </c>
       <c r="D35" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C36">
         <v>100</v>
       </c>
       <c r="D36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C37">
         <v>21</v>
       </c>
       <c r="D37" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B38" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C38">
         <v>30</v>
       </c>
       <c r="D38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C39">
         <v>5</v>
       </c>
       <c r="D39" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>323</v>
+      </c>
+      <c r="B40" t="s">
         <v>324</v>
-      </c>
-      <c r="B40" t="s">
-        <v>325</v>
       </c>
       <c r="C40">
         <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F40" s="14"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="36"/>
       <c r="B45" s="36"/>
       <c r="D45" s="36"/>
@@ -6487,690 +6487,690 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="41.5546875" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D1" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B3">
         <v>47.75</v>
       </c>
       <c r="C3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4">
         <v>1.83</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B5">
         <v>1.81</v>
       </c>
       <c r="C5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6">
         <v>1.81</v>
       </c>
       <c r="C6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B7">
         <v>1.5</v>
       </c>
       <c r="C7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="9">
         <v>0.28999999999999998</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9">
         <v>1.81</v>
       </c>
       <c r="C9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11">
         <v>49.26</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12">
         <v>1.18</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B13">
         <v>1.18</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14">
         <v>1.18</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B15">
         <v>1.53</v>
       </c>
       <c r="C15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B16">
         <v>1.18</v>
       </c>
       <c r="C16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B18">
         <v>1.51</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B19">
         <v>0.59</v>
       </c>
       <c r="C19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B20">
         <v>0.59</v>
       </c>
       <c r="C20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B21">
         <v>0.59</v>
       </c>
       <c r="C21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B22">
         <v>0.78</v>
       </c>
       <c r="C22" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B24">
         <v>0.59</v>
       </c>
       <c r="C24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B26" t="s">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D26" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>343</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B28">
         <v>17.420000000000002</v>
       </c>
       <c r="C28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D28" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B29">
         <v>1.18</v>
       </c>
       <c r="C29" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30">
         <v>1.18</v>
       </c>
       <c r="C30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B31">
         <v>0.81</v>
       </c>
       <c r="C31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B32">
         <v>0.39</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D32" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B33" s="9">
         <v>1.81</v>
       </c>
       <c r="C33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B34">
         <v>1.18</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B36">
         <v>1.71</v>
       </c>
       <c r="C36" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D36" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B37">
         <v>0.81</v>
       </c>
       <c r="C37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B38">
         <v>0.81</v>
       </c>
       <c r="C38" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D38" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B39">
         <v>0.81</v>
       </c>
       <c r="C39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40">
         <v>0.39</v>
       </c>
       <c r="C40" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D40" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B41">
         <v>1.81</v>
       </c>
       <c r="C41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B43">
         <v>1.63</v>
       </c>
       <c r="C43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B44">
         <v>0.81</v>
       </c>
       <c r="C44" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D44" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B45">
         <v>0.81</v>
       </c>
       <c r="C45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B46">
         <v>0.81</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B47">
         <v>0.38</v>
       </c>
       <c r="C47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C48" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B49">
         <v>0.81</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>369</v>
+      </c>
+      <c r="B55" t="s">
+        <v>370</v>
+      </c>
+      <c r="D55" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>372</v>
+      </c>
+      <c r="B56" t="s">
+        <v>371</v>
+      </c>
+      <c r="D56" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>376</v>
+      </c>
+      <c r="B57" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>370</v>
-      </c>
-      <c r="B55" t="s">
-        <v>371</v>
-      </c>
-      <c r="D55" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>373</v>
-      </c>
-      <c r="B56" t="s">
-        <v>372</v>
-      </c>
-      <c r="D56" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>377</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>375</v>
-      </c>
-      <c r="D57" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
figure making for the presentation ahoy
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63A532A-9A32-4947-A9B5-2D0E799741C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663DAD74-12E5-45EA-BBDC-AE6430D0E692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" firstSheet="1" activeTab="5" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="3" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -1997,20 +1997,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>7621</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>297180</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:rowOff>129541</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Afbeelding 2">
+        <xdr:cNvPr id="2" name="Afbeelding 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73BF72F1-A39F-77C5-C4C3-058057AD9B3C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D791AFC4-AF57-AB56-B0BF-3105F203DCF5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2018,21 +2018,16 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect r="38134" b="4215"/>
-        <a:stretch/>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="396240"/>
-          <a:ext cx="4686300" cy="6766560"/>
+          <a:off x="0" y="556261"/>
+          <a:ext cx="6233160" cy="6888480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2049,15 +2044,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>11429</xdr:rowOff>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>100524</xdr:rowOff>
+      <xdr:colOff>572366</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>89095</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2085,8 +2080,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="582929"/>
-          <a:ext cx="10410825" cy="15976795"/>
+          <a:off x="277091" y="0"/>
+          <a:ext cx="10700039" cy="14885750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2684,22 +2679,22 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="102.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="102.109375" customWidth="1"/>
+    <col min="3" max="3" width="61.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="7" max="7" width="32.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2719,7 +2714,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="109.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35" t="s">
         <v>267</v>
       </c>
@@ -2731,7 +2726,7 @@
       </c>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>57</v>
       </c>
@@ -2747,7 +2742,7 @@
       <c r="E3" s="7"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="33" t="s">
         <v>59</v>
       </c>
@@ -2763,7 +2758,7 @@
       <c r="E4" s="7"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="33" t="s">
         <v>64</v>
       </c>
@@ -2779,7 +2774,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="33" t="s">
         <v>67</v>
       </c>
@@ -2797,7 +2792,7 @@
       </c>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="33" t="s">
         <v>70</v>
       </c>
@@ -2813,7 +2808,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>74</v>
       </c>
@@ -2829,7 +2824,7 @@
       <c r="E8" s="7"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="33" t="s">
         <v>77</v>
       </c>
@@ -2847,7 +2842,7 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>82</v>
       </c>
@@ -2863,7 +2858,7 @@
       <c r="E10" s="7"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
@@ -2881,7 +2876,7 @@
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2899,7 +2894,7 @@
       </c>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -2915,7 +2910,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
@@ -2931,7 +2926,7 @@
       <c r="E14" s="7"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
@@ -2949,7 +2944,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -2965,7 +2960,7 @@
       <c r="E16" s="7"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>33</v>
       </c>
@@ -2981,7 +2976,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:9" ht="112.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
@@ -2997,7 +2992,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:9" ht="82.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>30</v>
       </c>
@@ -3015,7 +3010,7 @@
       </c>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>31</v>
       </c>
@@ -3033,7 +3028,7 @@
       </c>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:9" ht="97.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>53</v>
       </c>
@@ -3051,7 +3046,7 @@
       </c>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:9" ht="91.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -3071,7 +3066,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="101.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>51</v>
       </c>
@@ -3089,7 +3084,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:9" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -3107,7 +3102,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="67.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>49</v>
       </c>
@@ -3125,7 +3120,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
@@ -3146,7 +3141,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>235</v>
       </c>
@@ -3169,7 +3164,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -3180,7 +3175,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -3191,7 +3186,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -3202,7 +3197,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -3213,7 +3208,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -3224,7 +3219,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -3235,7 +3230,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -3246,7 +3241,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -3257,7 +3252,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="13"/>
     </row>
-    <row r="36" spans="1:9" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -3268,7 +3263,7 @@
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -3279,7 +3274,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="13"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -3290,7 +3285,7 @@
       <c r="H38" s="13"/>
       <c r="I38" s="13"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -3301,7 +3296,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -3312,7 +3307,7 @@
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -3323,7 +3318,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="13"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -3334,7 +3329,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -3345,7 +3340,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -3356,7 +3351,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -3367,7 +3362,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -3378,7 +3373,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -3389,7 +3384,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -3400,7 +3395,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -3411,7 +3406,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -3422,7 +3417,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -3433,7 +3428,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -3444,8 +3439,8 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -3456,7 +3451,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -3467,7 +3462,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -3478,8 +3473,8 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -3490,7 +3485,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -3501,7 +3496,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -3512,8 +3507,8 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -3524,7 +3519,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -3535,7 +3530,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -3546,7 +3541,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -3557,8 +3552,8 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -3569,7 +3564,7 @@
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -3580,7 +3575,7 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -3591,7 +3586,7 @@
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -3602,7 +3597,7 @@
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -3613,7 +3608,7 @@
       <c r="H71" s="13"/>
       <c r="I71" s="13"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -3624,7 +3619,7 @@
       <c r="H72" s="13"/>
       <c r="I72" s="13"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -3635,7 +3630,7 @@
       <c r="H73" s="13"/>
       <c r="I73" s="13"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -3646,7 +3641,7 @@
       <c r="H74" s="13"/>
       <c r="I74" s="13"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -3657,7 +3652,7 @@
       <c r="H75" s="13"/>
       <c r="I75" s="13"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -3668,7 +3663,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -3679,7 +3674,7 @@
       <c r="H77" s="13"/>
       <c r="I77" s="13"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -3690,7 +3685,7 @@
       <c r="H78" s="13"/>
       <c r="I78" s="13"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -3701,7 +3696,7 @@
       <c r="H79" s="13"/>
       <c r="I79" s="13"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -3712,7 +3707,7 @@
       <c r="H80" s="13"/>
       <c r="I80" s="13"/>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -3723,7 +3718,7 @@
       <c r="H81" s="13"/>
       <c r="I81" s="13"/>
     </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -3734,7 +3729,7 @@
       <c r="H82" s="13"/>
       <c r="I82" s="13"/>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -3759,7 +3754,7 @@
       <c r="V83" s="13"/>
       <c r="W83" s="13"/>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -3784,7 +3779,7 @@
       <c r="V84" s="13"/>
       <c r="W84" s="13"/>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -3809,7 +3804,7 @@
       <c r="V85" s="13"/>
       <c r="W85" s="13"/>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -3834,7 +3829,7 @@
       <c r="V86" s="13"/>
       <c r="W86" s="13"/>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A87" s="32"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -3859,7 +3854,7 @@
       <c r="V87" s="13"/>
       <c r="W87" s="13"/>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -3884,7 +3879,7 @@
       <c r="V88" s="13"/>
       <c r="W88" s="13"/>
     </row>
-    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -3909,7 +3904,7 @@
       <c r="V89" s="13"/>
       <c r="W89" s="13"/>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -3934,7 +3929,7 @@
       <c r="V90" s="13"/>
       <c r="W90" s="13"/>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -3959,7 +3954,7 @@
       <c r="V91" s="13"/>
       <c r="W91" s="13"/>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -3984,7 +3979,7 @@
       <c r="V92" s="13"/>
       <c r="W92" s="13"/>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -4009,7 +4004,7 @@
       <c r="V93" s="13"/>
       <c r="W93" s="13"/>
     </row>
-    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -4034,7 +4029,7 @@
       <c r="V94" s="13"/>
       <c r="W94" s="13"/>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -4059,7 +4054,7 @@
       <c r="V95" s="13"/>
       <c r="W95" s="13"/>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -4101,17 +4096,17 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" customWidth="1"/>
-    <col min="3" max="3" width="108.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="56.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.109375" customWidth="1"/>
+    <col min="2" max="2" width="62.109375" customWidth="1"/>
+    <col min="3" max="3" width="108.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4131,14 +4126,14 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>251</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
@@ -4152,7 +4147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -4166,7 +4161,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -4180,7 +4175,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -4197,7 +4192,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -4211,7 +4206,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -4225,7 +4220,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -4242,7 +4237,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>98</v>
       </c>
@@ -4256,13 +4251,13 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>250</v>
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -4279,7 +4274,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -4296,7 +4291,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>106</v>
       </c>
@@ -4310,7 +4305,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>108</v>
       </c>
@@ -4327,7 +4322,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>111</v>
       </c>
@@ -4344,7 +4339,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>114</v>
       </c>
@@ -4358,7 +4353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -4372,7 +4367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -4386,7 +4381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -4406,7 +4401,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -4423,13 +4418,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>247</v>
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -4446,7 +4441,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="87.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>126</v>
       </c>
@@ -4466,7 +4461,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -4483,7 +4478,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>131</v>
       </c>
@@ -4497,7 +4492,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>130</v>
       </c>
@@ -4511,7 +4506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="92.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -4525,7 +4520,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>235</v>
       </c>
@@ -4545,7 +4540,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>230</v>
       </c>
@@ -4553,7 +4548,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>232</v>
       </c>
@@ -4561,12 +4556,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -4577,12 +4572,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>239</v>
       </c>
@@ -4593,7 +4588,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>240</v>
       </c>
@@ -4616,20 +4611,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4649,17 +4644,17 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>351</v>
       </c>
@@ -4679,7 +4674,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>363</v>
       </c>
@@ -4696,7 +4691,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>362</v>
       </c>
@@ -4710,7 +4705,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>361</v>
       </c>
@@ -4737,21 +4732,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865D0B40-9BC0-4E55-824F-A8C0062232E1}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -4771,17 +4766,17 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>347</v>
       </c>
@@ -4801,7 +4796,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>353</v>
       </c>
@@ -4818,7 +4813,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>357</v>
       </c>
@@ -4832,7 +4827,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>355</v>
       </c>
@@ -4846,17 +4841,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>366</v>
       </c>
@@ -4878,17 +4873,17 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="54.33203125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4908,7 +4903,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -4922,7 +4917,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>271</v>
       </c>
@@ -4930,7 +4925,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -4941,7 +4936,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -4952,7 +4947,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -4963,7 +4958,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>284</v>
       </c>
@@ -4974,7 +4969,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>283</v>
       </c>
@@ -4985,7 +4980,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>282</v>
       </c>
@@ -4996,7 +4991,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -5007,7 +5002,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>280</v>
       </c>
@@ -5018,12 +5013,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -5037,7 +5032,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>296</v>
       </c>
@@ -5051,7 +5046,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>295</v>
       </c>
@@ -5065,7 +5060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>294</v>
       </c>
@@ -5079,7 +5074,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>293</v>
       </c>
@@ -5093,7 +5088,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>292</v>
       </c>
@@ -5107,7 +5102,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -5124,7 +5119,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>290</v>
       </c>
@@ -5144,7 +5139,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
         <v>263</v>
       </c>
@@ -5154,7 +5149,7 @@
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
     </row>
-    <row r="22" spans="1:6" ht="294.60000000000002" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="294.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>155</v>
       </c>
@@ -5185,21 +5180,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC645DA-818E-45E2-9276-0EC59E1A8287}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.85546875" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -5219,7 +5214,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>269</v>
       </c>
@@ -5236,7 +5231,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>271</v>
       </c>
@@ -5244,7 +5239,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>286</v>
       </c>
@@ -5258,7 +5253,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -5272,7 +5267,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -5286,7 +5281,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>284</v>
       </c>
@@ -5300,7 +5295,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>283</v>
       </c>
@@ -5314,7 +5309,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>282</v>
       </c>
@@ -5328,7 +5323,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>281</v>
       </c>
@@ -5342,7 +5337,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>280</v>
       </c>
@@ -5356,12 +5351,12 @@
         <v>258</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>297</v>
       </c>
@@ -5378,7 +5373,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>296</v>
       </c>
@@ -5395,7 +5390,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>295</v>
       </c>
@@ -5412,7 +5407,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>294</v>
       </c>
@@ -5429,7 +5424,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>293</v>
       </c>
@@ -5446,7 +5441,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>292</v>
       </c>
@@ -5463,7 +5458,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>291</v>
       </c>
@@ -5483,7 +5478,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="130.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>235</v>
       </c>
@@ -5503,7 +5498,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="345" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>155</v>
       </c>
@@ -5537,18 +5532,18 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5569,7 +5564,7 @@
       </c>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>248</v>
       </c>
@@ -5578,7 +5573,7 @@
       </c>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5597,7 +5592,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -5616,7 +5611,7 @@
       <c r="F4" s="3"/>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:7" ht="97.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5634,7 +5629,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:7" ht="79.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5652,7 +5647,7 @@
       </c>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:7" ht="182.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -5671,7 +5666,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -5690,7 +5685,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="30"/>
     </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -5705,7 +5700,7 @@
       </c>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:7" ht="169.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>249</v>
       </c>
@@ -5714,11 +5709,11 @@
       </c>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:7" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5739,7 +5734,7 @@
       </c>
       <c r="G12" s="30"/>
     </row>
-    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -5760,13 +5755,13 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:7" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G15" s="30"/>
     </row>
-    <row r="16" spans="1:7" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="30"/>
       <c r="B16" s="30"/>
       <c r="C16" s="30"/>
@@ -5775,7 +5770,7 @@
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="30"/>
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
@@ -5800,15 +5795,15 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -5828,7 +5823,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>303</v>
       </c>
@@ -5838,7 +5833,7 @@
       <c r="E2" s="18"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" ht="116.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>160</v>
       </c>
@@ -5856,7 +5851,7 @@
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row r="4" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>163</v>
       </c>
@@ -5874,7 +5869,7 @@
       </c>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>167</v>
       </c>
@@ -5892,7 +5887,7 @@
       </c>
       <c r="F5" s="15"/>
     </row>
-    <row r="6" spans="1:6" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>168</v>
       </c>
@@ -5910,7 +5905,7 @@
       </c>
       <c r="F6" s="14"/>
     </row>
-    <row r="7" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
         <v>169</v>
       </c>
@@ -5928,7 +5923,7 @@
       </c>
       <c r="F7" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>170</v>
       </c>
@@ -5946,7 +5941,7 @@
       </c>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>171</v>
       </c>
@@ -5964,7 +5959,7 @@
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row r="10" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
         <v>172</v>
       </c>
@@ -5982,7 +5977,7 @@
       </c>
       <c r="F10" s="14"/>
     </row>
-    <row r="11" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>173</v>
       </c>
@@ -6000,7 +5995,7 @@
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>174</v>
       </c>
@@ -6018,7 +6013,7 @@
       </c>
       <c r="F12" s="14"/>
     </row>
-    <row r="13" spans="1:6" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>243</v>
       </c>
@@ -6036,7 +6031,7 @@
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>175</v>
       </c>
@@ -6054,7 +6049,7 @@
       </c>
       <c r="F14" s="14"/>
     </row>
-    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>244</v>
       </c>
@@ -6072,7 +6067,7 @@
       </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
         <v>177</v>
       </c>
@@ -6090,7 +6085,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="1:6" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>179</v>
       </c>
@@ -6108,7 +6103,7 @@
       </c>
       <c r="F17" s="15"/>
     </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
         <v>180</v>
       </c>
@@ -6126,7 +6121,7 @@
       </c>
       <c r="F18" s="14"/>
     </row>
-    <row r="19" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>182</v>
       </c>
@@ -6144,7 +6139,7 @@
       </c>
       <c r="F19" s="15"/>
     </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
         <v>183</v>
       </c>
@@ -6162,17 +6157,17 @@
       </c>
       <c r="F20" s="26"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>304</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E23" s="28"/>
     </row>
-    <row r="24" spans="1:6" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>305</v>
       </c>
@@ -6190,7 +6185,7 @@
       </c>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>163</v>
       </c>
@@ -6207,7 +6202,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>309</v>
       </c>
@@ -6225,7 +6220,7 @@
       </c>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>310</v>
       </c>
@@ -6242,7 +6237,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>312</v>
       </c>
@@ -6260,7 +6255,7 @@
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>313</v>
       </c>
@@ -6277,7 +6272,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>314</v>
       </c>
@@ -6295,7 +6290,7 @@
       </c>
       <c r="F30" s="14"/>
     </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>315</v>
       </c>
@@ -6312,7 +6307,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>316</v>
       </c>
@@ -6330,7 +6325,7 @@
       </c>
       <c r="F32" s="14"/>
     </row>
-    <row r="33" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>317</v>
       </c>
@@ -6347,7 +6342,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>318</v>
       </c>
@@ -6365,7 +6360,7 @@
       </c>
       <c r="F34" s="14"/>
     </row>
-    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>307</v>
       </c>
@@ -6382,7 +6377,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>319</v>
       </c>
@@ -6400,7 +6395,7 @@
       </c>
       <c r="F36" s="14"/>
     </row>
-    <row r="37" spans="1:6" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>320</v>
       </c>
@@ -6417,7 +6412,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>321</v>
       </c>
@@ -6435,7 +6430,7 @@
       </c>
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>322</v>
       </c>
@@ -6452,7 +6447,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>323</v>
       </c>
@@ -6470,7 +6465,7 @@
       </c>
       <c r="F40" s="14"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="36"/>
       <c r="B45" s="36"/>
       <c r="D45" s="36"/>
@@ -6491,15 +6486,15 @@
       <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>229</v>
       </c>
@@ -6513,7 +6508,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="100.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>339</v>
       </c>
@@ -6521,7 +6516,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>215</v>
       </c>
@@ -6535,7 +6530,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>213</v>
       </c>
@@ -6549,7 +6544,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>211</v>
       </c>
@@ -6563,7 +6558,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>209</v>
       </c>
@@ -6577,7 +6572,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>207</v>
       </c>
@@ -6591,7 +6586,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>205</v>
       </c>
@@ -6605,7 +6600,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>202</v>
       </c>
@@ -6619,7 +6614,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>340</v>
       </c>
@@ -6627,7 +6622,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -6641,7 +6636,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>213</v>
       </c>
@@ -6655,7 +6650,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>211</v>
       </c>
@@ -6669,7 +6664,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>209</v>
       </c>
@@ -6683,7 +6678,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>207</v>
       </c>
@@ -6697,7 +6692,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>202</v>
       </c>
@@ -6711,7 +6706,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A17" s="39" t="s">
         <v>377</v>
       </c>
@@ -6719,7 +6714,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -6733,7 +6728,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>213</v>
       </c>
@@ -6747,7 +6742,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>211</v>
       </c>
@@ -6761,7 +6756,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>209</v>
       </c>
@@ -6775,7 +6770,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>207</v>
       </c>
@@ -6789,7 +6784,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>205</v>
       </c>
@@ -6803,7 +6798,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>202</v>
       </c>
@@ -6817,7 +6812,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>229</v>
       </c>
@@ -6831,7 +6826,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>342</v>
       </c>
@@ -6839,7 +6834,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -6853,7 +6848,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>213</v>
       </c>
@@ -6867,7 +6862,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>211</v>
       </c>
@@ -6881,7 +6876,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -6895,7 +6890,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>207</v>
       </c>
@@ -6909,7 +6904,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -6923,7 +6918,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>202</v>
       </c>
@@ -6937,7 +6932,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>343</v>
       </c>
@@ -6945,7 +6940,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>215</v>
       </c>
@@ -6959,7 +6954,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>213</v>
       </c>
@@ -6973,7 +6968,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>211</v>
       </c>
@@ -6987,7 +6982,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>209</v>
       </c>
@@ -7001,7 +6996,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>207</v>
       </c>
@@ -7015,7 +7010,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>202</v>
       </c>
@@ -7029,7 +7024,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="39" t="s">
         <v>378</v>
       </c>
@@ -7037,7 +7032,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -7051,7 +7046,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>213</v>
       </c>
@@ -7065,7 +7060,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>211</v>
       </c>
@@ -7079,7 +7074,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>209</v>
       </c>
@@ -7093,7 +7088,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>207</v>
       </c>
@@ -7107,7 +7102,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>205</v>
       </c>
@@ -7121,7 +7116,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>202</v>
       </c>
@@ -7135,12 +7130,12 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>369</v>
       </c>
@@ -7151,7 +7146,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>372</v>
       </c>
@@ -7162,7 +7157,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>376</v>
       </c>

</xml_diff>

<commit_message>
finishing up the report
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41207D9B-C98B-4642-B5B9-593A07DC77DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C19FB-3F85-4052-B10A-ED8AF504F3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="3" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" firstSheet="1" activeTab="5" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Kasteel population" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="385">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -1464,10 +1464,22 @@
     <t>Benzaldehyde Rat (Wrong)</t>
   </si>
   <si>
+    <t>A value of 245 umol/kg is noted in the paper</t>
+  </si>
+  <si>
+    <t>http://xnet.hsl.gov.uk/Popgen/input.aspx</t>
+  </si>
+  <si>
+    <t>Kothari A, Rajagopalan P. The assembly of integrated rat intestinal-hepatocyte cultures. Bioeng Transl Med. 2019 Nov 9;5(1):e10146. doi: 10.1002/btm2.10146. PMID: 31989035; PMCID: PMC6971435.</t>
+  </si>
+  <si>
+    <t>Herbert F Helander &amp; Lars Fändriks (2014) Surface area of the digestive tract – revisited, Scandinavian Journal of Gastroenterology, 49:6, 681-689, DOI: 10.3109/00365521.2014.898326</t>
+  </si>
+  <si>
     <t>#Calculation of Ka and Fa based on the QSAR in Ans Punt
 #Just change h polar sufrace area
 Human
-R&lt;-0.4 #radius small intestine = C/2π=2.52·π≈0.39789cm
+R&lt;-1.25 radius small intestine =2.50/2≈1.26cm
 Tsi&lt;-1.63 #small intestine transit time 
 kt&lt;-1/(Tsi/7)
 #Polar surface area
@@ -1483,7 +1495,7 @@
     <t>#Calculation of Ka and Fa based on the QSAR in Ans Punt
 #Just change h polar surface area
 #rat
-R&lt;-0.18 #radius small intestine
+R&lt;-0.126 #radius small intestine 0.252/2
 Tsi&lt;-1.63 #small intestine transit time 
 kt&lt;-1/(Tsi/7)
 #Polar surface area
@@ -1495,18 +1507,12 @@
 Ka= (Peff.cm.per.hr*2)/R
 Fa = 1-(1+Ka/kt)**-7</t>
   </si>
-  <si>
-    <t>A value of 245 umol/kg is noted in the paper</t>
-  </si>
-  <si>
-    <t>http://xnet.hsl.gov.uk/Popgen/input.aspx</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1586,6 +1592,19 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1671,19 +1690,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1703,95 +1719,53 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{DE7BC18A-9D54-48A0-AB30-07C48903A88E}"/>
     <cellStyle name="Standard 2" xfId="2" xr:uid="{8BE6A642-AF34-43F4-A01E-4F8E076EA935}"/>
   </cellStyles>
   <dxfs count="19">
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="5" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1885,6 +1859,44 @@
         <bottom style="thin">
           <color theme="5" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="5"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="5" tint="0.39997558519241921"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -2277,22 +2289,23 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}" name="Tabel9" displayName="Tabel9" ref="A1:F45" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="A1:F45" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}" name="Tabel9" displayName="Tabel9" ref="A1:G45" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:G45" xr:uid="{171F60C9-1D7F-4413-B0D6-77DEA07E7496}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E56BCEE8-B1D6-4C01-83D0-DDF02E730936}" name="Parameter "/>
     <tableColumn id="2" xr3:uid="{96282FD4-2AB5-46C0-84E6-07A379FF044E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{802A6005-6357-486B-8C9A-87BF2F885998}" name="Value"/>
     <tableColumn id="4" xr3:uid="{615BC5FA-61AF-4462-875E-E04F892B0E9F}" name="Unit "/>
     <tableColumn id="5" xr3:uid="{C7F31ACE-1EBB-427A-91F5-E41C9C93CF90}" name="Reference "/>
     <tableColumn id="6" xr3:uid="{1C2F99DB-227A-49AA-8974-75E712C3A56D}" name="Notes"/>
+    <tableColumn id="7" xr3:uid="{294EE942-E7AE-46F5-B9AF-7973A3269C0F}" name="http://xnet.hsl.gov.uk/Popgen/input.aspx"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}" name="Tabel911" displayName="Tabel911" ref="A1:F47" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}" name="Tabel911" displayName="Tabel911" ref="A1:F47" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:F47" xr:uid="{51E08D91-F477-4C86-B179-14637CAC9E0F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{0E284C69-B1DD-4E31-A3F5-7CB96E6AF19D}" name="Parameter "/>
@@ -2352,15 +2365,15 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}" name="Tabel3" displayName="Tabel3" ref="A1:F40" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}" name="Tabel3" displayName="Tabel3" ref="A1:F40" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:F40" xr:uid="{CDD00638-1865-4903-A605-FED7957B54E7}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9E6D16AC-BCC0-4871-B66F-97BF63950B51}" name="Parameter "/>
     <tableColumn id="2" xr3:uid="{26DD8215-41B0-459C-A9AE-2F2D7AFDB86E}" name="Description"/>
     <tableColumn id="3" xr3:uid="{14CB4CA6-E35E-4F7D-A582-7A40DA32B9E0}" name="Value"/>
     <tableColumn id="4" xr3:uid="{5EBB9576-9587-4C7D-A236-37CEF71F24E3}" name="Unit "/>
-    <tableColumn id="5" xr3:uid="{EA1BF9BF-3C1D-47A0-98E2-6A086009FE82}" name="Reference " dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{2D8D3B4C-6456-4490-A06B-05F8F69E5369}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{EA1BF9BF-3C1D-47A0-98E2-6A086009FE82}" name="Reference " dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{2D8D3B4C-6456-4490-A06B-05F8F69E5369}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2697,1390 +2710,1390 @@
     <col min="13" max="13" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="109.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="70.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:9" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:9" ht="112.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="82.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:9" ht="81.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:9" ht="97.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:9" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="67.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="3" t="s">
+      <c r="E25" s="5"/>
+      <c r="F25" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="3" t="s">
+      <c r="E26" s="5"/>
+      <c r="F26" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" ht="72" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>265</v>
       </c>
       <c r="C27" t="s">
         <v>241</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" ht="216" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="13"/>
-      <c r="D58" s="13"/>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="13"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13"/>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="13"/>
-      <c r="D60" s="13"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-    </row>
-    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="13"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-    </row>
-    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3"/>
+      <c r="A65" s="10"/>
+      <c r="B65" s="10"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
+      <c r="A67" s="10"/>
+      <c r="B67" s="10"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
+      <c r="A68" s="10"/>
+      <c r="B68" s="10"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="13"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="13"/>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
+      <c r="A69" s="10"/>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13"/>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
+      <c r="A70" s="10"/>
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="13"/>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
+      <c r="A71" s="10"/>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="13"/>
-      <c r="D72" s="13"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="13"/>
-      <c r="D73" s="13"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
+      <c r="A73" s="10"/>
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="13"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="13"/>
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
+      <c r="A74" s="10"/>
+      <c r="B74" s="10"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="13"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="13"/>
-      <c r="D75" s="13"/>
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
+      <c r="A75" s="10"/>
+      <c r="B75" s="10"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="13"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="13"/>
-      <c r="D76" s="13"/>
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
+      <c r="A76" s="10"/>
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="13"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="13"/>
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
+      <c r="A77" s="10"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="13"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="13"/>
-      <c r="D78" s="13"/>
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
+      <c r="A78" s="10"/>
+      <c r="B78" s="10"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="13"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="13"/>
-      <c r="D79" s="13"/>
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
+      <c r="A79" s="10"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="13"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="13"/>
-      <c r="D80" s="13"/>
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
+      <c r="A80" s="10"/>
+      <c r="B80" s="10"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A81" s="13"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="13"/>
-      <c r="D81" s="13"/>
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
+      <c r="A81" s="10"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A82" s="13"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="10"/>
+      <c r="C82" s="10"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A83" s="13"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="13"/>
-      <c r="D83" s="13"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
-      <c r="K83" s="13"/>
-      <c r="L83" s="13"/>
-      <c r="M83" s="13"/>
-      <c r="N83" s="13"/>
-      <c r="O83" s="13"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="13"/>
-      <c r="R83" s="13"/>
-      <c r="S83" s="13"/>
-      <c r="T83" s="13"/>
-      <c r="U83" s="13"/>
-      <c r="V83" s="13"/>
-      <c r="W83" s="13"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="10"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
+      <c r="L83" s="10"/>
+      <c r="M83" s="10"/>
+      <c r="N83" s="10"/>
+      <c r="O83" s="10"/>
+      <c r="P83" s="10"/>
+      <c r="Q83" s="10"/>
+      <c r="R83" s="10"/>
+      <c r="S83" s="10"/>
+      <c r="T83" s="10"/>
+      <c r="U83" s="10"/>
+      <c r="V83" s="10"/>
+      <c r="W83" s="10"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A84" s="13"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="13"/>
-      <c r="D84" s="13"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
-      <c r="K84" s="13"/>
-      <c r="L84" s="13"/>
-      <c r="M84" s="13"/>
-      <c r="N84" s="13"/>
-      <c r="O84" s="13"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="13"/>
-      <c r="R84" s="13"/>
-      <c r="S84" s="13"/>
-      <c r="T84" s="13"/>
-      <c r="U84" s="13"/>
-      <c r="V84" s="13"/>
-      <c r="W84" s="13"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="10"/>
+      <c r="C84" s="10"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
+      <c r="L84" s="10"/>
+      <c r="M84" s="10"/>
+      <c r="N84" s="10"/>
+      <c r="O84" s="10"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="10"/>
+      <c r="R84" s="10"/>
+      <c r="S84" s="10"/>
+      <c r="T84" s="10"/>
+      <c r="U84" s="10"/>
+      <c r="V84" s="10"/>
+      <c r="W84" s="10"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A85" s="13"/>
-      <c r="B85" s="13"/>
-      <c r="C85" s="13"/>
-      <c r="D85" s="13"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
-      <c r="K85" s="13"/>
-      <c r="L85" s="13"/>
-      <c r="M85" s="13"/>
-      <c r="N85" s="13"/>
-      <c r="O85" s="13"/>
-      <c r="P85" s="13"/>
-      <c r="Q85" s="13"/>
-      <c r="R85" s="13"/>
-      <c r="S85" s="13"/>
-      <c r="T85" s="13"/>
-      <c r="U85" s="13"/>
-      <c r="V85" s="13"/>
-      <c r="W85" s="13"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
+      <c r="L85" s="10"/>
+      <c r="M85" s="10"/>
+      <c r="N85" s="10"/>
+      <c r="O85" s="10"/>
+      <c r="P85" s="10"/>
+      <c r="Q85" s="10"/>
+      <c r="R85" s="10"/>
+      <c r="S85" s="10"/>
+      <c r="T85" s="10"/>
+      <c r="U85" s="10"/>
+      <c r="V85" s="10"/>
+      <c r="W85" s="10"/>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A86" s="13"/>
-      <c r="B86" s="13"/>
-      <c r="C86" s="13"/>
-      <c r="D86" s="13"/>
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
-      <c r="K86" s="13"/>
-      <c r="L86" s="13"/>
-      <c r="M86" s="13"/>
-      <c r="N86" s="13"/>
-      <c r="O86" s="13"/>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="13"/>
-      <c r="R86" s="13"/>
-      <c r="S86" s="13"/>
-      <c r="T86" s="13"/>
-      <c r="U86" s="13"/>
-      <c r="V86" s="13"/>
-      <c r="W86" s="13"/>
+      <c r="A86" s="10"/>
+      <c r="B86" s="10"/>
+      <c r="C86" s="10"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="10"/>
+      <c r="L86" s="10"/>
+      <c r="M86" s="10"/>
+      <c r="N86" s="10"/>
+      <c r="O86" s="10"/>
+      <c r="P86" s="10"/>
+      <c r="Q86" s="10"/>
+      <c r="R86" s="10"/>
+      <c r="S86" s="10"/>
+      <c r="T86" s="10"/>
+      <c r="U86" s="10"/>
+      <c r="V86" s="10"/>
+      <c r="W86" s="10"/>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A87" s="32"/>
-      <c r="B87" s="13"/>
-      <c r="C87" s="13"/>
-      <c r="D87" s="13"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
-      <c r="K87" s="13"/>
-      <c r="L87" s="13"/>
-      <c r="M87" s="13"/>
-      <c r="N87" s="13"/>
-      <c r="O87" s="13"/>
-      <c r="P87" s="13"/>
-      <c r="Q87" s="13"/>
-      <c r="R87" s="13"/>
-      <c r="S87" s="13"/>
-      <c r="T87" s="13"/>
-      <c r="U87" s="13"/>
-      <c r="V87" s="13"/>
-      <c r="W87" s="13"/>
+      <c r="A87" s="27"/>
+      <c r="B87" s="10"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10"/>
+      <c r="L87" s="10"/>
+      <c r="M87" s="10"/>
+      <c r="N87" s="10"/>
+      <c r="O87" s="10"/>
+      <c r="P87" s="10"/>
+      <c r="Q87" s="10"/>
+      <c r="R87" s="10"/>
+      <c r="S87" s="10"/>
+      <c r="T87" s="10"/>
+      <c r="U87" s="10"/>
+      <c r="V87" s="10"/>
+      <c r="W87" s="10"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A88" s="13"/>
-      <c r="B88" s="13"/>
-      <c r="C88" s="13"/>
-      <c r="D88" s="13"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
-      <c r="K88" s="13"/>
-      <c r="L88" s="13"/>
-      <c r="M88" s="13"/>
-      <c r="N88" s="13"/>
-      <c r="O88" s="13"/>
-      <c r="P88" s="13"/>
-      <c r="Q88" s="13"/>
-      <c r="R88" s="13"/>
-      <c r="S88" s="13"/>
-      <c r="T88" s="13"/>
-      <c r="U88" s="13"/>
-      <c r="V88" s="13"/>
-      <c r="W88" s="13"/>
+      <c r="A88" s="10"/>
+      <c r="B88" s="10"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
+      <c r="L88" s="10"/>
+      <c r="M88" s="10"/>
+      <c r="N88" s="10"/>
+      <c r="O88" s="10"/>
+      <c r="P88" s="10"/>
+      <c r="Q88" s="10"/>
+      <c r="R88" s="10"/>
+      <c r="S88" s="10"/>
+      <c r="T88" s="10"/>
+      <c r="U88" s="10"/>
+      <c r="V88" s="10"/>
+      <c r="W88" s="10"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A89" s="13"/>
-      <c r="B89" s="13"/>
-      <c r="C89" s="13"/>
-      <c r="D89" s="13"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
-      <c r="M89" s="13"/>
-      <c r="N89" s="13"/>
-      <c r="O89" s="13"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="13"/>
-      <c r="R89" s="13"/>
-      <c r="S89" s="13"/>
-      <c r="T89" s="13"/>
-      <c r="U89" s="13"/>
-      <c r="V89" s="13"/>
-      <c r="W89" s="13"/>
+      <c r="A89" s="10"/>
+      <c r="B89" s="10"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+      <c r="S89" s="10"/>
+      <c r="T89" s="10"/>
+      <c r="U89" s="10"/>
+      <c r="V89" s="10"/>
+      <c r="W89" s="10"/>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A90" s="13"/>
-      <c r="B90" s="13"/>
-      <c r="C90" s="13"/>
-      <c r="D90" s="13"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
-      <c r="M90" s="13"/>
-      <c r="N90" s="13"/>
-      <c r="O90" s="13"/>
-      <c r="P90" s="13"/>
-      <c r="Q90" s="13"/>
-      <c r="R90" s="13"/>
-      <c r="S90" s="13"/>
-      <c r="T90" s="13"/>
-      <c r="U90" s="13"/>
-      <c r="V90" s="13"/>
-      <c r="W90" s="13"/>
+      <c r="A90" s="10"/>
+      <c r="B90" s="10"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
+      <c r="L90" s="10"/>
+      <c r="M90" s="10"/>
+      <c r="N90" s="10"/>
+      <c r="O90" s="10"/>
+      <c r="P90" s="10"/>
+      <c r="Q90" s="10"/>
+      <c r="R90" s="10"/>
+      <c r="S90" s="10"/>
+      <c r="T90" s="10"/>
+      <c r="U90" s="10"/>
+      <c r="V90" s="10"/>
+      <c r="W90" s="10"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A91" s="13"/>
-      <c r="B91" s="13"/>
-      <c r="C91" s="13"/>
-      <c r="D91" s="13"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
-      <c r="M91" s="13"/>
-      <c r="N91" s="13"/>
-      <c r="O91" s="13"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="13"/>
-      <c r="R91" s="13"/>
-      <c r="S91" s="13"/>
-      <c r="T91" s="13"/>
-      <c r="U91" s="13"/>
-      <c r="V91" s="13"/>
-      <c r="W91" s="13"/>
+      <c r="A91" s="10"/>
+      <c r="B91" s="10"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
+      <c r="L91" s="10"/>
+      <c r="M91" s="10"/>
+      <c r="N91" s="10"/>
+      <c r="O91" s="10"/>
+      <c r="P91" s="10"/>
+      <c r="Q91" s="10"/>
+      <c r="R91" s="10"/>
+      <c r="S91" s="10"/>
+      <c r="T91" s="10"/>
+      <c r="U91" s="10"/>
+      <c r="V91" s="10"/>
+      <c r="W91" s="10"/>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A92" s="13"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="13"/>
-      <c r="D92" s="13"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
-      <c r="M92" s="13"/>
-      <c r="N92" s="13"/>
-      <c r="O92" s="13"/>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="13"/>
-      <c r="R92" s="13"/>
-      <c r="S92" s="13"/>
-      <c r="T92" s="13"/>
-      <c r="U92" s="13"/>
-      <c r="V92" s="13"/>
-      <c r="W92" s="13"/>
+      <c r="A92" s="10"/>
+      <c r="B92" s="10"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
+      <c r="L92" s="10"/>
+      <c r="M92" s="10"/>
+      <c r="N92" s="10"/>
+      <c r="O92" s="10"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+      <c r="S92" s="10"/>
+      <c r="T92" s="10"/>
+      <c r="U92" s="10"/>
+      <c r="V92" s="10"/>
+      <c r="W92" s="10"/>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A93" s="13"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="13"/>
-      <c r="D93" s="13"/>
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
-      <c r="M93" s="13"/>
-      <c r="N93" s="13"/>
-      <c r="O93" s="13"/>
-      <c r="P93" s="13"/>
-      <c r="Q93" s="13"/>
-      <c r="R93" s="13"/>
-      <c r="S93" s="13"/>
-      <c r="T93" s="13"/>
-      <c r="U93" s="13"/>
-      <c r="V93" s="13"/>
-      <c r="W93" s="13"/>
+      <c r="A93" s="10"/>
+      <c r="B93" s="10"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
+      <c r="L93" s="10"/>
+      <c r="M93" s="10"/>
+      <c r="N93" s="10"/>
+      <c r="O93" s="10"/>
+      <c r="P93" s="10"/>
+      <c r="Q93" s="10"/>
+      <c r="R93" s="10"/>
+      <c r="S93" s="10"/>
+      <c r="T93" s="10"/>
+      <c r="U93" s="10"/>
+      <c r="V93" s="10"/>
+      <c r="W93" s="10"/>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A94" s="13"/>
-      <c r="B94" s="13"/>
-      <c r="C94" s="13"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
-      <c r="M94" s="13"/>
-      <c r="N94" s="13"/>
-      <c r="O94" s="13"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="13"/>
-      <c r="R94" s="13"/>
-      <c r="S94" s="13"/>
-      <c r="T94" s="13"/>
-      <c r="U94" s="13"/>
-      <c r="V94" s="13"/>
-      <c r="W94" s="13"/>
+      <c r="A94" s="10"/>
+      <c r="B94" s="10"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
+      <c r="L94" s="10"/>
+      <c r="M94" s="10"/>
+      <c r="N94" s="10"/>
+      <c r="O94" s="10"/>
+      <c r="P94" s="10"/>
+      <c r="Q94" s="10"/>
+      <c r="R94" s="10"/>
+      <c r="S94" s="10"/>
+      <c r="T94" s="10"/>
+      <c r="U94" s="10"/>
+      <c r="V94" s="10"/>
+      <c r="W94" s="10"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A95" s="13"/>
-      <c r="B95" s="13"/>
-      <c r="C95" s="13"/>
-      <c r="D95" s="13"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="13"/>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13"/>
-      <c r="K95" s="13"/>
-      <c r="L95" s="13"/>
-      <c r="M95" s="13"/>
-      <c r="N95" s="13"/>
-      <c r="O95" s="13"/>
-      <c r="P95" s="13"/>
-      <c r="Q95" s="13"/>
-      <c r="R95" s="13"/>
-      <c r="S95" s="13"/>
-      <c r="T95" s="13"/>
-      <c r="U95" s="13"/>
-      <c r="V95" s="13"/>
-      <c r="W95" s="13"/>
+      <c r="A95" s="10"/>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
+      <c r="L95" s="10"/>
+      <c r="M95" s="10"/>
+      <c r="N95" s="10"/>
+      <c r="O95" s="10"/>
+      <c r="P95" s="10"/>
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10"/>
+      <c r="S95" s="10"/>
+      <c r="T95" s="10"/>
+      <c r="U95" s="10"/>
+      <c r="V95" s="10"/>
+      <c r="W95" s="10"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="13"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
-      <c r="M96" s="13"/>
-      <c r="N96" s="13"/>
-      <c r="O96" s="13"/>
-      <c r="P96" s="13"/>
-      <c r="Q96" s="13"/>
-      <c r="R96" s="13"/>
-      <c r="S96" s="13"/>
-      <c r="T96" s="13"/>
-      <c r="U96" s="13"/>
-      <c r="V96" s="13"/>
-      <c r="W96" s="13"/>
+      <c r="A96" s="10"/>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="10"/>
+      <c r="L96" s="10"/>
+      <c r="M96" s="10"/>
+      <c r="N96" s="10"/>
+      <c r="O96" s="10"/>
+      <c r="P96" s="10"/>
+      <c r="Q96" s="10"/>
+      <c r="R96" s="10"/>
+      <c r="S96" s="10"/>
+      <c r="T96" s="10"/>
+      <c r="U96" s="10"/>
+      <c r="V96" s="10"/>
+      <c r="W96" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4130,17 +4143,17 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C3" t="s">
@@ -4227,7 +4240,7 @@
       <c r="A9" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>94</v>
       </c>
       <c r="C9" t="s">
@@ -4247,7 +4260,7 @@
       <c r="B10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>97</v>
       </c>
       <c r="D10" t="s">
@@ -4255,10 +4268,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -4273,7 +4285,7 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>187</v>
       </c>
     </row>
@@ -4290,7 +4302,7 @@
       <c r="D13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4321,7 +4333,7 @@
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4338,7 +4350,7 @@
       <c r="D16" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4397,10 +4409,10 @@
       <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="4" t="s">
         <v>191</v>
       </c>
     </row>
@@ -4417,15 +4429,15 @@
       <c r="D21" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -4457,10 +4469,10 @@
       <c r="D24" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4477,7 +4489,7 @@
       <c r="D25" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="5" t="s">
         <v>193</v>
       </c>
     </row>
@@ -4536,10 +4548,10 @@
       <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -4614,8 +4626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E614F67-C4E8-46C8-8B4D-B73636AD116D}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4628,26 +4640,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="30" t="s">
         <v>259</v>
       </c>
-      <c r="G1" t="s">
-        <v>382</v>
+      <c r="G1" s="33" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -4664,7 +4676,7 @@
       <c r="A42" t="s">
         <v>351</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>234</v>
       </c>
       <c r="C42" t="s">
@@ -4673,10 +4685,10 @@
       <c r="D42" t="s">
         <v>35</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4687,13 +4699,13 @@
       <c r="B43" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>358</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4726,10 +4738,13 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G1" r:id="rId1" xr:uid="{7D344849-D07A-4706-8685-F3B3F1C8E517}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4738,7 +4753,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865D0B40-9BC0-4E55-824F-A8C0062232E1}">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
@@ -4753,26 +4768,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="30" t="s">
         <v>259</v>
       </c>
       <c r="I1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -4789,7 +4804,7 @@
       <c r="A42" t="s">
         <v>347</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>234</v>
       </c>
       <c r="C42" t="s">
@@ -4798,10 +4813,10 @@
       <c r="D42" t="s">
         <v>35</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F42" s="2" t="s">
         <v>350</v>
       </c>
     </row>
@@ -4812,13 +4827,13 @@
       <c r="B43" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>352</v>
       </c>
       <c r="D43" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4878,8 +4893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA63B1E-9727-458D-B78C-352DAEF35D45}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4893,22 +4908,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>259</v>
       </c>
     </row>
@@ -4927,7 +4942,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>271</v>
       </c>
       <c r="D3" t="s">
@@ -5023,7 +5038,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5124,7 +5139,7 @@
       <c r="D19" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>298</v>
       </c>
     </row>
@@ -5141,40 +5156,37 @@
       <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="1:6" ht="294.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:6" ht="308.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>155</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C22">
-        <v>1.37</v>
+        <v>1.97</v>
       </c>
       <c r="D22" t="s">
         <v>198</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="F22" s="3"/>
+      <c r="E22" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>381</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5189,8 +5201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC645DA-818E-45E2-9276-0EC59E1A8287}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5199,27 +5211,27 @@
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" customWidth="1"/>
+    <col min="5" max="5" width="42.77734375" customWidth="1"/>
     <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="10" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5236,12 +5248,12 @@
       <c r="D2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>271</v>
       </c>
       <c r="D3" t="s">
@@ -5361,7 +5373,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="8" t="s">
         <v>287</v>
       </c>
     </row>
@@ -5483,47 +5495,49 @@
       <c r="E19" t="s">
         <v>258</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>265</v>
       </c>
       <c r="C20">
         <v>540</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="322.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>155</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C21">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="D21" t="s">
         <v>198</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="F21" s="34" t="s">
+        <v>382</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5535,9 +5549,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227D4F3-7485-4534-9D8C-979B86ED3B4D}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -5552,7 +5566,7 @@
     <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5571,18 +5585,16 @@
       <c r="F1" t="s">
         <v>259</v>
       </c>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>136</v>
       </c>
@@ -5595,13 +5607,12 @@
       <c r="D3" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="30"/>
-    </row>
-    <row r="4" spans="1:7" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -5614,13 +5625,12 @@
       <c r="D4" t="s">
         <v>133</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="30"/>
-    </row>
-    <row r="5" spans="1:7" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -5633,12 +5643,11 @@
       <c r="D5" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" spans="1:7" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -5651,12 +5660,11 @@
       <c r="D6" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="1:7" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -5669,13 +5677,12 @@
       <c r="D7" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="30"/>
-    </row>
-    <row r="8" spans="1:7" ht="174" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>146</v>
       </c>
@@ -5688,17 +5695,16 @@
       <c r="D8" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="30"/>
-    </row>
-    <row r="9" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>147</v>
       </c>
       <c r="C9" t="s">
@@ -5707,22 +5713,19 @@
       <c r="D9" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:7" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+    </row>
+    <row r="10" spans="1:6" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:7" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -5735,15 +5738,14 @@
       <c r="D12" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:7" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>152</v>
       </c>
@@ -5756,38 +5758,16 @@
       <c r="D13" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="G13" s="30"/>
-    </row>
-    <row r="14" spans="1:7" ht="87" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:7" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G15" s="30"/>
-    </row>
-    <row r="16" spans="1:7" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-    </row>
+      <c r="F13" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5798,9 +5778,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC505D8B-0BF3-4962-BD98-F6AA5F552AB5}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -5813,368 +5793,368 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="21" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="12">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>8.5</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>330</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F5" s="15"/>
+      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="11">
         <v>100</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="19">
         <v>100</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="11">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>73</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F9" s="15"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="11">
         <v>37</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="19">
         <v>100</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="11">
         <v>70</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>90</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E13" s="28" t="s">
+      <c r="E13" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="11">
         <v>290</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="19">
         <v>600</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F15" s="15"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="11">
         <v>100</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>21</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="11">
         <v>30</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>5</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="25" t="s">
         <v>258</v>
       </c>
-      <c r="F19" s="15"/>
+      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="22">
         <v>63</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F20" s="26"/>
+      <c r="F20" s="23"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="28"/>
+      <c r="E23" s="25"/>
     </row>
     <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -6189,10 +6169,10 @@
       <c r="D24" t="s">
         <v>325</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
@@ -6207,7 +6187,7 @@
       <c r="D25" t="s">
         <v>245</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6224,10 +6204,10 @@
       <c r="D26" t="s">
         <v>245</v>
       </c>
-      <c r="E26" s="27" t="s">
+      <c r="E26" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="11"/>
     </row>
     <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -6242,7 +6222,7 @@
       <c r="D27" t="s">
         <v>245</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6259,10 +6239,10 @@
       <c r="D28" t="s">
         <v>245</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="11"/>
     </row>
     <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
@@ -6277,7 +6257,7 @@
       <c r="D29" t="s">
         <v>325</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6294,10 +6274,10 @@
       <c r="D30" t="s">
         <v>325</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="11"/>
     </row>
     <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -6312,7 +6292,7 @@
       <c r="D31" t="s">
         <v>325</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6329,10 +6309,10 @@
       <c r="D32" t="s">
         <v>245</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="11"/>
     </row>
     <row r="33" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -6347,7 +6327,7 @@
       <c r="D33" t="s">
         <v>245</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6364,10 +6344,10 @@
       <c r="D34" t="s">
         <v>245</v>
       </c>
-      <c r="E34" s="27" t="s">
+      <c r="E34" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="11"/>
     </row>
     <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
@@ -6382,7 +6362,7 @@
       <c r="D35" t="s">
         <v>245</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6399,10 +6379,10 @@
       <c r="D36" t="s">
         <v>245</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
@@ -6417,7 +6397,7 @@
       <c r="D37" t="s">
         <v>325</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6434,10 +6414,10 @@
       <c r="D38" t="s">
         <v>325</v>
       </c>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
@@ -6452,7 +6432,7 @@
       <c r="D39" t="s">
         <v>325</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="E39" s="25" t="s">
         <v>258</v>
       </c>
     </row>
@@ -6469,15 +6449,10 @@
       <c r="D40" t="s">
         <v>325</v>
       </c>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="F40" s="14"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="D45" s="36"/>
+      <c r="F40" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6491,8 +6466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6518,10 +6493,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6535,7 +6510,7 @@
       <c r="C3" t="s">
         <v>227</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6549,7 +6524,7 @@
       <c r="C4" t="s">
         <v>226</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6563,7 +6538,7 @@
       <c r="C5" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6577,7 +6552,7 @@
       <c r="C6" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6591,7 +6566,7 @@
       <c r="C7" t="s">
         <v>223</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6599,13 +6574,13 @@
       <c r="A8" t="s">
         <v>205</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>0.28999999999999998</v>
       </c>
       <c r="C8" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6619,15 +6594,15 @@
       <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>340</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6641,7 +6616,7 @@
       <c r="C11" t="s">
         <v>221</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6655,7 +6630,7 @@
       <c r="C12" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6669,7 +6644,7 @@
       <c r="C13" t="s">
         <v>219</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6683,7 +6658,7 @@
       <c r="C14" t="s">
         <v>218</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6697,7 +6672,7 @@
       <c r="C15" t="s">
         <v>217</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6711,15 +6686,15 @@
       <c r="C16" t="s">
         <v>216</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="31" t="s">
         <v>377</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6733,7 +6708,7 @@
       <c r="C18" t="s">
         <v>214</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6747,7 +6722,7 @@
       <c r="C19" t="s">
         <v>212</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6761,7 +6736,7 @@
       <c r="C20" t="s">
         <v>210</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6775,7 +6750,7 @@
       <c r="C21" t="s">
         <v>208</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6789,7 +6764,7 @@
       <c r="C22" t="s">
         <v>206</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6797,13 +6772,13 @@
       <c r="A23" t="s">
         <v>205</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>204</v>
       </c>
       <c r="C23" t="s">
         <v>203</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6817,7 +6792,7 @@
       <c r="C24" t="s">
         <v>201</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6836,10 +6811,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6853,7 +6828,7 @@
       <c r="C28" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6867,7 +6842,7 @@
       <c r="C29" t="s">
         <v>226</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6881,7 +6856,7 @@
       <c r="C30" t="s">
         <v>225</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6895,7 +6870,7 @@
       <c r="C31" t="s">
         <v>224</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6909,7 +6884,7 @@
       <c r="C32" t="s">
         <v>223</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6917,13 +6892,13 @@
       <c r="A33" t="s">
         <v>205</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <v>1.81</v>
       </c>
       <c r="C33" t="s">
         <v>222</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -6937,15 +6912,15 @@
       <c r="C34" t="s">
         <v>201</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="2" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -6959,7 +6934,7 @@
       <c r="C36" t="s">
         <v>221</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6973,7 +6948,7 @@
       <c r="C37" t="s">
         <v>220</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -6987,7 +6962,7 @@
       <c r="C38" t="s">
         <v>219</v>
       </c>
-      <c r="D38" s="29" t="s">
+      <c r="D38" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7001,7 +6976,7 @@
       <c r="C39" t="s">
         <v>218</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7015,7 +6990,7 @@
       <c r="C40" t="s">
         <v>217</v>
       </c>
-      <c r="D40" s="29" t="s">
+      <c r="D40" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7029,15 +7004,15 @@
       <c r="C41" t="s">
         <v>216</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="6" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="31" t="s">
         <v>378</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>261</v>
       </c>
     </row>
@@ -7051,7 +7026,7 @@
       <c r="C43" t="s">
         <v>214</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7065,7 +7040,7 @@
       <c r="C44" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7079,7 +7054,7 @@
       <c r="C45" t="s">
         <v>210</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7093,7 +7068,7 @@
       <c r="C46" t="s">
         <v>208</v>
       </c>
-      <c r="D46" s="29" t="s">
+      <c r="D46" s="26" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7107,7 +7082,7 @@
       <c r="C47" t="s">
         <v>206</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="6" t="s">
         <v>262</v>
       </c>
     </row>
@@ -7115,13 +7090,13 @@
       <c r="A48" t="s">
         <v>205</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="7" t="s">
         <v>204</v>
       </c>
       <c r="C48" t="s">
         <v>203</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>260</v>
       </c>
     </row>
@@ -7135,7 +7110,7 @@
       <c r="C49" t="s">
         <v>201</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="2" t="s">
         <v>261</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added more calculation for single rat an human. and some other minor changes
</commit_message>
<xml_diff>
--- a/Parameter supplementary data.xlsx
+++ b/Parameter supplementary data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86A980A-41D3-4A2B-96AD-83D26330DDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF1BDDE-5838-489C-9504-3DA347F90B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="860" activeTab="4" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="860" activeTab="6" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Male Popgen" sheetId="6" r:id="rId1"/>
@@ -894,7 +894,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1997,16 +1997,16 @@
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2029,17 +2029,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="177" customHeight="1">
+    <row r="42" spans="1:6" ht="177" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>194</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="150">
+    <row r="43" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>206</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>205</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>204</v>
       </c>
@@ -2124,17 +2124,17 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -2157,17 +2157,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="171" customHeight="1">
+    <row r="42" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>190</v>
       </c>
@@ -2187,7 +2187,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="135">
+    <row r="43" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>196</v>
       </c>
@@ -2204,7 +2204,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>200</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>198</v>
       </c>
@@ -2232,17 +2232,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="3:3">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="59" spans="3:3">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="61" spans="3:3">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
         <v>209</v>
       </c>
@@ -2264,17 +2264,17 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="54.33203125" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2338,7 +2338,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>5.6</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2404,12 +2404,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="102.6" customHeight="1">
+    <row r="20" spans="1:6" ht="102.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>133</v>
       </c>
@@ -2530,12 +2530,12 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="308.25" customHeight="1">
+    <row r="22" spans="1:6" ht="308.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2572,17 +2572,17 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="42.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="119.45" customHeight="1">
+    <row r="2" spans="1:6" ht="119.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>112</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>127</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>124</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -2739,12 +2739,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>137</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>135</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>134</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="130.15" customHeight="1">
+    <row r="20" spans="1:6" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>92</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="322.89999999999998" customHeight="1">
+    <row r="21" spans="1:6" ht="322.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -2918,22 +2918,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C227D4F3-7485-4534-9D8C-979B86ED3B4D}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="56.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="72.28515625" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="72.33203125" customWidth="1"/>
+    <col min="6" max="6" width="41.109375" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +2953,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="180.6" customHeight="1">
+    <row r="2" spans="1:6" ht="180.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="165" customHeight="1">
+    <row r="3" spans="1:6" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -2979,7 +2979,7 @@
       </c>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" ht="132.6" customHeight="1">
+    <row r="4" spans="1:6" ht="132.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2997,7 +2997,7 @@
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="97.9" customHeight="1">
+    <row r="5" spans="1:6" ht="97.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="79.900000000000006" customHeight="1">
+    <row r="6" spans="1:6" ht="79.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="182.45" customHeight="1">
+    <row r="7" spans="1:6" ht="182.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="174" customHeight="1">
+    <row r="8" spans="1:6" ht="174" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1">
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="169.15" customHeight="1">
+    <row r="10" spans="1:6" ht="169.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>98</v>
       </c>
@@ -3089,10 +3089,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="43.15" customHeight="1">
+    <row r="11" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="117.6" customHeight="1">
+    <row r="12" spans="1:6" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="120.6" customHeight="1">
+    <row r="13" spans="1:6" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -3132,9 +3132,9 @@
         <v>212</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="87" customHeight="1"/>
-    <row r="15" spans="1:6" ht="142.15" customHeight="1"/>
-    <row r="16" spans="1:6" ht="22.15" customHeight="1"/>
+    <row r="14" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3151,15 +3151,15 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" customWidth="1"/>
+    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3179,7 +3179,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>146</v>
       </c>
@@ -3189,7 +3189,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
     </row>
-    <row r="3" spans="1:6" ht="116.45" customHeight="1">
+    <row r="3" spans="1:6" ht="116.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>39</v>
       </c>
@@ -3207,7 +3207,7 @@
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="1:6" ht="22.9" customHeight="1">
+    <row r="4" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>42</v>
       </c>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" spans="1:6" ht="26.45" customHeight="1">
+    <row r="5" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>46</v>
       </c>
@@ -3243,7 +3243,7 @@
       </c>
       <c r="F5" s="11"/>
     </row>
-    <row r="6" spans="1:6" ht="62.45" customHeight="1">
+    <row r="6" spans="1:6" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>47</v>
       </c>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" spans="1:6" ht="22.15" customHeight="1">
+    <row r="7" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>48</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="1:6" ht="24.6" customHeight="1">
+    <row r="8" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>49</v>
       </c>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" spans="1:6" ht="23.45" customHeight="1">
+    <row r="9" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>50</v>
       </c>
@@ -3315,7 +3315,7 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="23.45" customHeight="1">
+    <row r="10" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>51</v>
       </c>
@@ -3333,7 +3333,7 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" spans="1:6" ht="22.9" customHeight="1">
+    <row r="11" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>52</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" ht="21.6" customHeight="1">
+    <row r="12" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>53</v>
       </c>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="19.149999999999999" customHeight="1">
+    <row r="13" spans="1:6" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>93</v>
       </c>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="1:6" ht="23.45" customHeight="1">
+    <row r="14" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>54</v>
       </c>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1">
+    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>94</v>
       </c>
@@ -3423,7 +3423,7 @@
       </c>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="1:6" ht="22.15" customHeight="1">
+    <row r="16" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>56</v>
       </c>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" ht="23.45" customHeight="1">
+    <row r="17" spans="1:6" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>58</v>
       </c>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1">
+    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>59</v>
       </c>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" spans="1:6" ht="22.15" customHeight="1">
+    <row r="19" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>61</v>
       </c>
@@ -3495,7 +3495,7 @@
       </c>
       <c r="F19" s="11"/>
     </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1">
+    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>62</v>
       </c>
@@ -3513,17 +3513,17 @@
       </c>
       <c r="F20" s="20"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>147</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="19.899999999999999" customHeight="1">
+    <row r="24" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>148</v>
       </c>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="F24" s="10"/>
     </row>
-    <row r="25" spans="1:6" ht="24.6" customHeight="1">
+    <row r="25" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="21" customHeight="1">
+    <row r="26" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>152</v>
       </c>
@@ -3576,7 +3576,7 @@
       </c>
       <c r="F26" s="10"/>
     </row>
-    <row r="27" spans="1:6" ht="27" customHeight="1">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>153</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24.6" customHeight="1">
+    <row r="28" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>155</v>
       </c>
@@ -3611,7 +3611,7 @@
       </c>
       <c r="F28" s="10"/>
     </row>
-    <row r="29" spans="1:6" ht="24" customHeight="1">
+    <row r="29" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>156</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24.6" customHeight="1">
+    <row r="30" spans="1:6" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>157</v>
       </c>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="F30" s="10"/>
     </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1">
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>158</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="22.15" customHeight="1">
+    <row r="32" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>159</v>
       </c>
@@ -3681,7 +3681,7 @@
       </c>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6" ht="25.9" customHeight="1">
+    <row r="33" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>160</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="22.15" customHeight="1">
+    <row r="34" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>161</v>
       </c>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="F34" s="10"/>
     </row>
-    <row r="35" spans="1:6" ht="21" customHeight="1">
+    <row r="35" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>150</v>
       </c>
@@ -3733,7 +3733,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="25.9" customHeight="1">
+    <row r="36" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>162</v>
       </c>
@@ -3751,7 +3751,7 @@
       </c>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" ht="26.45" customHeight="1">
+    <row r="37" spans="1:6" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>163</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="22.9" customHeight="1">
+    <row r="38" spans="1:6" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -3786,7 +3786,7 @@
       </c>
       <c r="F38" s="10"/>
     </row>
-    <row r="39" spans="1:6" ht="25.9" customHeight="1">
+    <row r="39" spans="1:6" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>165</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="36.6" customHeight="1">
+    <row r="40" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>166</v>
       </c>
@@ -3833,19 +3833,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B715CF8A-5161-4A0C-964A-ED7D03D4C131}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -3859,7 +3859,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="100.9" customHeight="1">
+    <row r="2" spans="1:4" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>182</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -3881,7 +3881,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>73</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="135">
+    <row r="8" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>71</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="105">
+    <row r="9" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="105">
+    <row r="10" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>183</v>
       </c>
@@ -3973,7 +3973,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -3987,7 +3987,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>75</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>73</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -4043,7 +4043,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -4057,33 +4057,33 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="26"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D19" s="23"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D21" s="23"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" s="6"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>90</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105">
+    <row r="27" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>185</v>
       </c>
@@ -4105,7 +4105,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>76</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -4175,7 +4175,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="135">
+    <row r="33" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="105">
+    <row r="34" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>70</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="105">
+    <row r="35" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>186</v>
       </c>
@@ -4211,7 +4211,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>76</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>73</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -4295,30 +4295,30 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="26"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D44" s="23"/>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D45" s="5"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D46" s="23"/>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D47" s="5"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B48" s="6"/>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" s="1"/>
     </row>
   </sheetData>

</xml_diff>